<commit_message>
checking collinearity - init knotscheme
</commit_message>
<xml_diff>
--- a/data/0_traits/birdTraits-merged-all.xlsx
+++ b/data/0_traits/birdTraits-merged-all.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhr597/Library/CloudStorage/Box-Box/PhD/projects/hmsc-danishbirds/data/0_traits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7303518-A0E0-8F48-A02E-6C14CFE44472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522DF7F5-3FC7-104A-B420-0C8D01EAC05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{0978E254-0241-384A-8752-F99CA5CCCD90}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3988" uniqueCount="1116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3989" uniqueCount="1116">
   <si>
     <t>X</t>
   </si>
@@ -4272,11 +4272,11 @@
   <dimension ref="A1:AH229"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="V206" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="AG1" sqref="AG1:AG1048576"/>
+      <selection pane="bottomRight" activeCell="T150" sqref="T150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4284,6 +4284,7 @@
     <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.83203125" customWidth="1"/>
     <col min="16" max="16" width="10.83203125" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
     <col min="18" max="18" width="33.83203125" bestFit="1" customWidth="1"/>
@@ -17176,9 +17177,8 @@
       <c r="R149" t="s">
         <v>719</v>
       </c>
-      <c r="U149" t="str">
-        <f t="shared" si="4"/>
-        <v>Terrestrial and low¬† flycatching feeders</v>
+      <c r="U149" t="s">
+        <v>675</v>
       </c>
       <c r="V149">
         <v>0</v>

</xml_diff>

<commit_message>
fixed mistakes related to traits
</commit_message>
<xml_diff>
--- a/data/0_traits/birdTraits-merged-all.xlsx
+++ b/data/0_traits/birdTraits-merged-all.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhr597/Library/CloudStorage/Box-Box/PhD/projects/hmsc-danishbirds/data/0_traits/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/1883199306832/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522DF7F5-3FC7-104A-B420-0C8D01EAC05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -4272,11 +4272,11 @@
   <dimension ref="A1:AH229"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O129" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="T150" sqref="T150"/>
+      <selection pane="bottomRight" activeCell="R141" sqref="R141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
edited taxonomy and things
</commit_message>
<xml_diff>
--- a/data/0_traits/birdTraits-merged-all.xlsx
+++ b/data/0_traits/birdTraits-merged-all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/1883199306832/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="661" documentId="13_ncr:1_{522DF7F5-3FC7-104A-B420-0C8D01EAC05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{046E3E5C-59B9-B84E-92FB-70AA33F5AF6B}"/>
+  <xr:revisionPtr revIDLastSave="673" documentId="13_ncr:1_{522DF7F5-3FC7-104A-B420-0C8D01EAC05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E480A06-88E6-D444-BC92-6BC08F6040D5}"/>
   <bookViews>
-    <workbookView xWindow="18440" yWindow="760" windowWidth="29540" windowHeight="18880" xr2:uid="{0978E254-0241-384A-8752-F99CA5CCCD90}"/>
+    <workbookView xWindow="700" yWindow="760" windowWidth="29540" windowHeight="17820" xr2:uid="{0978E254-0241-384A-8752-F99CA5CCCD90}"/>
   </bookViews>
   <sheets>
     <sheet name="birdTraits-merged" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4375" uniqueCount="1101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4376" uniqueCount="1102">
   <si>
     <t>X</t>
   </si>
@@ -3366,6 +3366,9 @@
   </si>
   <si>
     <t>Count of Migration_a3_DOF_description</t>
+  </si>
+  <si>
+    <t>rare_quant</t>
   </si>
 </sst>
 </file>
@@ -5085,6 +5088,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Wessel Mulder" refreshedDate="45903.575466550923" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="229" xr:uid="{59ABAB41-0182-C543-8F04-C6635D12F12C}">
   <cacheSource type="worksheet">
@@ -5804,7 +5811,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AC06D153-7537-594C-9220-42EEFD1FD5AE}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AC06D153-7537-594C-9220-42EEFD1FD5AE}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0" sortType="ascending">
@@ -6258,14 +6265,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{848F7BD8-942D-B14D-BC97-3359E0D31A09}">
-  <dimension ref="A1:BS229"/>
+  <dimension ref="A1:BT229"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="111" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="L159" sqref="L159"/>
+      <selection pane="bottomRight" activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6289,7 +6296,7 @@
     <col min="28" max="28" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:72" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8"/>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -6379,13 +6386,16 @@
         <v>1051</v>
       </c>
       <c r="AE1" s="8" t="s">
+        <v>1101</v>
+      </c>
+      <c r="AF1" s="8" t="s">
         <v>1052</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AG1" s="9" t="s">
         <v>1092</v>
       </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>48</v>
       </c>
@@ -6476,9 +6486,16 @@
       <c r="AB2" s="6"/>
       <c r="AC2" s="6"/>
       <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-    </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE2" s="6" t="str">
+        <f>IF(V2&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF2" s="6"/>
+      <c r="AG2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>50</v>
       </c>
@@ -6567,9 +6584,13 @@
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-    </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE3" s="6" t="str">
+        <f>IF(V3&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF3" s="6"/>
+    </row>
+    <row r="4" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>47</v>
       </c>
@@ -6660,9 +6681,13 @@
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
-      <c r="AE4" s="6"/>
-    </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE4" s="6" t="str">
+        <f>IF(V4&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF4" s="6"/>
+    </row>
+    <row r="5" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>49</v>
       </c>
@@ -6753,9 +6778,13 @@
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-    </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE5" s="6" t="str">
+        <f>IF(V5&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF5" s="6"/>
+    </row>
+    <row r="6" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>44</v>
       </c>
@@ -6844,9 +6873,13 @@
       <c r="AB6" s="6"/>
       <c r="AC6" s="6"/>
       <c r="AD6" s="6"/>
-      <c r="AE6" s="6"/>
-    </row>
-    <row r="7" spans="1:71" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE6" s="6" t="str">
+        <f>IF(V6&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF6" s="6"/>
+    </row>
+    <row r="7" spans="1:72" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>45</v>
       </c>
@@ -6935,8 +6968,11 @@
       <c r="AB7" s="6"/>
       <c r="AC7" s="6"/>
       <c r="AD7" s="6"/>
-      <c r="AE7" s="6"/>
-      <c r="AF7"/>
+      <c r="AE7" s="6" t="str">
+        <f>IF(V7&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF7" s="6"/>
       <c r="AG7"/>
       <c r="AH7"/>
       <c r="AI7"/>
@@ -6976,8 +7012,9 @@
       <c r="BQ7"/>
       <c r="BR7"/>
       <c r="BS7"/>
-    </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT7"/>
+    </row>
+    <row r="8" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>46</v>
       </c>
@@ -7068,9 +7105,13 @@
       <c r="AB8" s="6"/>
       <c r="AC8" s="6"/>
       <c r="AD8" s="6"/>
-      <c r="AE8" s="6"/>
-    </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE8" s="6" t="str">
+        <f>IF(V8&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF8" s="6"/>
+    </row>
+    <row r="9" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>43</v>
       </c>
@@ -7161,9 +7202,13 @@
       <c r="AB9" s="6"/>
       <c r="AC9" s="6"/>
       <c r="AD9" s="6"/>
-      <c r="AE9" s="6"/>
-    </row>
-    <row r="10" spans="1:71" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE9" s="6" t="str">
+        <f>IF(V9&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF9" s="6"/>
+    </row>
+    <row r="10" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>42</v>
       </c>
@@ -7254,8 +7299,11 @@
       <c r="AB10" s="6"/>
       <c r="AC10" s="6"/>
       <c r="AD10" s="6"/>
-      <c r="AE10" s="6"/>
-      <c r="AF10"/>
+      <c r="AE10" s="6" t="str">
+        <f>IF(V10&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF10" s="6"/>
       <c r="AG10"/>
       <c r="AH10"/>
       <c r="AI10"/>
@@ -7295,8 +7343,9 @@
       <c r="BQ10"/>
       <c r="BR10"/>
       <c r="BS10"/>
-    </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT10"/>
+    </row>
+    <row r="11" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>51</v>
       </c>
@@ -7385,9 +7434,13 @@
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
       <c r="AD11" s="6"/>
-      <c r="AE11" s="6"/>
-    </row>
-    <row r="12" spans="1:71" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE11" s="6" t="str">
+        <f>IF(V11&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF11" s="6"/>
+    </row>
+    <row r="12" spans="1:72" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>41</v>
       </c>
@@ -7476,8 +7529,11 @@
       <c r="AB12" s="6"/>
       <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
-      <c r="AE12" s="6"/>
-      <c r="AF12"/>
+      <c r="AE12" s="6" t="str">
+        <f>IF(V12&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF12" s="6"/>
       <c r="AG12"/>
       <c r="AH12"/>
       <c r="AI12"/>
@@ -7517,8 +7573,9 @@
       <c r="BQ12"/>
       <c r="BR12"/>
       <c r="BS12"/>
-    </row>
-    <row r="13" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT12"/>
+    </row>
+    <row r="13" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>23</v>
       </c>
@@ -7604,11 +7661,14 @@
         <v>1</v>
       </c>
       <c r="AD13" s="5"/>
-      <c r="AE13" s="5"/>
-      <c r="AF13" s="2">
+      <c r="AE13" s="5">
+        <f>IF(V13&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG13"/>
+      <c r="AF13" s="5"/>
+      <c r="AG13" s="2">
+        <v>1</v>
+      </c>
       <c r="AH13"/>
       <c r="AI13"/>
       <c r="AJ13"/>
@@ -7647,8 +7707,9 @@
       <c r="BQ13"/>
       <c r="BR13"/>
       <c r="BS13"/>
-    </row>
-    <row r="14" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT13"/>
+    </row>
+    <row r="14" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>20</v>
       </c>
@@ -7741,11 +7802,14 @@
         <v>1</v>
       </c>
       <c r="AD14" s="5"/>
-      <c r="AE14" s="5"/>
-      <c r="AF14" s="2">
+      <c r="AE14" s="5" t="str">
+        <f>IF(V14&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="2">
         <v>1</v>
       </c>
-      <c r="AG14"/>
       <c r="AH14"/>
       <c r="AI14"/>
       <c r="AJ14"/>
@@ -7784,8 +7848,9 @@
       <c r="BQ14"/>
       <c r="BR14"/>
       <c r="BS14"/>
-    </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT14"/>
+    </row>
+    <row r="15" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>28</v>
       </c>
@@ -7876,9 +7941,13 @@
       <c r="AB15" s="6"/>
       <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
-      <c r="AE15" s="6"/>
-    </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE15" s="6" t="str">
+        <f>IF(V15&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF15" s="6"/>
+    </row>
+    <row r="16" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>26</v>
       </c>
@@ -7967,9 +8036,13 @@
       <c r="AB16" s="6"/>
       <c r="AC16" s="6"/>
       <c r="AD16" s="6"/>
-      <c r="AE16" s="6"/>
-    </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE16" s="6" t="str">
+        <f>IF(V16&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF16" s="6"/>
+    </row>
+    <row r="17" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>27</v>
       </c>
@@ -8060,9 +8133,13 @@
       <c r="AB17" s="6"/>
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
-      <c r="AE17" s="6"/>
-    </row>
-    <row r="18" spans="1:71" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE17" s="6" t="str">
+        <f>IF(V17&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF17" s="6"/>
+    </row>
+    <row r="18" spans="1:72" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -8151,8 +8228,11 @@
       <c r="AB18" s="6"/>
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
-      <c r="AE18" s="6"/>
-      <c r="AF18"/>
+      <c r="AE18" s="6" t="str">
+        <f>IF(V18&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF18" s="6"/>
       <c r="AG18"/>
       <c r="AH18"/>
       <c r="AI18"/>
@@ -8192,8 +8272,9 @@
       <c r="BQ18"/>
       <c r="BR18"/>
       <c r="BS18"/>
-    </row>
-    <row r="19" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT18"/>
+    </row>
+    <row r="19" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -8286,11 +8367,14 @@
         <v>1</v>
       </c>
       <c r="AD19" s="5"/>
-      <c r="AE19" s="5"/>
-      <c r="AF19" s="2">
+      <c r="AE19" s="5">
+        <f>IF(V19&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG19"/>
+      <c r="AF19" s="5"/>
+      <c r="AG19" s="2">
+        <v>1</v>
+      </c>
       <c r="AH19"/>
       <c r="AI19"/>
       <c r="AJ19"/>
@@ -8329,8 +8413,9 @@
       <c r="BQ19"/>
       <c r="BR19"/>
       <c r="BS19"/>
-    </row>
-    <row r="20" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT19"/>
+    </row>
+    <row r="20" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>32</v>
       </c>
@@ -8421,9 +8506,13 @@
       <c r="AB20" s="6"/>
       <c r="AC20" s="6"/>
       <c r="AD20" s="6"/>
-      <c r="AE20" s="6"/>
-    </row>
-    <row r="21" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE20" s="6" t="str">
+        <f>IF(V20&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF20" s="6"/>
+    </row>
+    <row r="21" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>33</v>
       </c>
@@ -8514,8 +8603,11 @@
       <c r="AB21" s="6"/>
       <c r="AC21" s="6"/>
       <c r="AD21" s="6"/>
-      <c r="AE21" s="6"/>
-      <c r="AF21"/>
+      <c r="AE21" s="6" t="str">
+        <f>IF(V21&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF21" s="6"/>
       <c r="AG21"/>
       <c r="AH21"/>
       <c r="AI21"/>
@@ -8555,8 +8647,9 @@
       <c r="BQ21"/>
       <c r="BR21"/>
       <c r="BS21"/>
-    </row>
-    <row r="22" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT21"/>
+    </row>
+    <row r="22" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>34</v>
       </c>
@@ -8647,11 +8740,14 @@
       </c>
       <c r="AC22" s="5"/>
       <c r="AD22" s="5"/>
-      <c r="AE22" s="5"/>
-      <c r="AF22" s="2">
+      <c r="AE22" s="5">
+        <f>IF(V22&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG22"/>
+      <c r="AF22" s="5"/>
+      <c r="AG22" s="2">
+        <v>1</v>
+      </c>
       <c r="AH22"/>
       <c r="AI22"/>
       <c r="AJ22"/>
@@ -8690,8 +8786,9 @@
       <c r="BQ22"/>
       <c r="BR22"/>
       <c r="BS22"/>
-    </row>
-    <row r="23" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT22"/>
+    </row>
+    <row r="23" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>18</v>
       </c>
@@ -8786,11 +8883,14 @@
         <v>1</v>
       </c>
       <c r="AD23" s="5"/>
-      <c r="AE23" s="5"/>
-      <c r="AF23" s="2">
+      <c r="AE23" s="5" t="str">
+        <f>IF(V23&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF23" s="5"/>
+      <c r="AG23" s="2">
         <v>1</v>
       </c>
-      <c r="AG23"/>
       <c r="AH23"/>
       <c r="AI23"/>
       <c r="AJ23"/>
@@ -8829,8 +8929,9 @@
       <c r="BQ23"/>
       <c r="BR23"/>
       <c r="BS23"/>
-    </row>
-    <row r="24" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT23"/>
+    </row>
+    <row r="24" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>19</v>
       </c>
@@ -8921,8 +9022,11 @@
       <c r="AB24" s="6"/>
       <c r="AC24" s="6"/>
       <c r="AD24" s="6"/>
-      <c r="AE24" s="6"/>
-      <c r="AF24"/>
+      <c r="AE24" s="6" t="str">
+        <f>IF(V24&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF24" s="6"/>
       <c r="AG24"/>
       <c r="AH24"/>
       <c r="AI24"/>
@@ -8962,8 +9066,9 @@
       <c r="BQ24"/>
       <c r="BR24"/>
       <c r="BS24"/>
-    </row>
-    <row r="25" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT24"/>
+    </row>
+    <row r="25" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>37</v>
       </c>
@@ -9056,9 +9161,13 @@
       <c r="AB25" s="6"/>
       <c r="AC25" s="6"/>
       <c r="AD25" s="6"/>
-      <c r="AE25" s="6"/>
-    </row>
-    <row r="26" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE25" s="6" t="str">
+        <f>IF(V25&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF25" s="6"/>
+    </row>
+    <row r="26" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>36</v>
       </c>
@@ -9149,11 +9258,14 @@
       </c>
       <c r="AC26" s="5"/>
       <c r="AD26" s="5"/>
-      <c r="AE26" s="5"/>
-      <c r="AF26" s="2">
+      <c r="AE26" s="5">
+        <f>IF(V26&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG26"/>
+      <c r="AF26" s="5"/>
+      <c r="AG26" s="2">
+        <v>1</v>
+      </c>
       <c r="AH26"/>
       <c r="AI26"/>
       <c r="AJ26"/>
@@ -9192,8 +9304,9 @@
       <c r="BQ26"/>
       <c r="BR26"/>
       <c r="BS26"/>
-    </row>
-    <row r="27" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT26"/>
+    </row>
+    <row r="27" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>15</v>
       </c>
@@ -9282,9 +9395,13 @@
       <c r="AB27" s="6"/>
       <c r="AC27" s="6"/>
       <c r="AD27" s="6"/>
-      <c r="AE27" s="6"/>
-    </row>
-    <row r="28" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE27" s="6" t="str">
+        <f>IF(V27&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF27" s="6"/>
+    </row>
+    <row r="28" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>14</v>
       </c>
@@ -9375,9 +9492,13 @@
       <c r="AB28" s="6"/>
       <c r="AC28" s="6"/>
       <c r="AD28" s="6"/>
-      <c r="AE28" s="6"/>
-    </row>
-    <row r="29" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE28" s="6" t="str">
+        <f>IF(V28&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF28" s="6"/>
+    </row>
+    <row r="29" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>24</v>
       </c>
@@ -9468,9 +9589,13 @@
       <c r="AB29" s="6"/>
       <c r="AC29" s="6"/>
       <c r="AD29" s="6"/>
-      <c r="AE29" s="6"/>
-    </row>
-    <row r="30" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE29" s="6" t="str">
+        <f>IF(V29&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF29" s="6"/>
+    </row>
+    <row r="30" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>25</v>
       </c>
@@ -9561,9 +9686,13 @@
       <c r="AB30" s="6"/>
       <c r="AC30" s="6"/>
       <c r="AD30" s="6"/>
-      <c r="AE30" s="6"/>
-    </row>
-    <row r="31" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE30" s="6" t="str">
+        <f>IF(V30&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF30" s="6"/>
+    </row>
+    <row r="31" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>38</v>
       </c>
@@ -9654,11 +9783,14 @@
       </c>
       <c r="AC31" s="5"/>
       <c r="AD31" s="5"/>
-      <c r="AE31" s="5"/>
-      <c r="AF31" s="2">
+      <c r="AE31" s="5">
+        <f>IF(V31&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG31"/>
+      <c r="AF31" s="5"/>
+      <c r="AG31" s="2">
+        <v>1</v>
+      </c>
       <c r="AH31"/>
       <c r="AI31"/>
       <c r="AJ31"/>
@@ -9697,8 +9829,9 @@
       <c r="BQ31"/>
       <c r="BR31"/>
       <c r="BS31"/>
-    </row>
-    <row r="32" spans="1:71" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT31"/>
+    </row>
+    <row r="32" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>40</v>
       </c>
@@ -9789,8 +9922,11 @@
       <c r="AB32" s="6"/>
       <c r="AC32" s="6"/>
       <c r="AD32" s="6"/>
-      <c r="AE32" s="6"/>
-      <c r="AF32"/>
+      <c r="AE32" s="6" t="str">
+        <f>IF(V32&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF32" s="6"/>
       <c r="AG32"/>
       <c r="AH32"/>
       <c r="AI32"/>
@@ -9830,8 +9966,9 @@
       <c r="BQ32"/>
       <c r="BR32"/>
       <c r="BS32"/>
-    </row>
-    <row r="33" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT32"/>
+    </row>
+    <row r="33" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>39</v>
       </c>
@@ -9922,9 +10059,13 @@
       <c r="AB33" s="6"/>
       <c r="AC33" s="6"/>
       <c r="AD33" s="6"/>
-      <c r="AE33" s="6"/>
-    </row>
-    <row r="34" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE33" s="6" t="str">
+        <f>IF(V33&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF33" s="6"/>
+    </row>
+    <row r="34" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>31</v>
       </c>
@@ -10017,11 +10158,14 @@
       <c r="AD34" s="5">
         <v>1</v>
       </c>
-      <c r="AE34" s="5"/>
-      <c r="AF34" s="2">
+      <c r="AE34" s="5" t="str">
+        <f>IF(V34&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF34" s="5"/>
+      <c r="AG34" s="2">
         <v>1</v>
       </c>
-      <c r="AG34"/>
       <c r="AH34"/>
       <c r="AI34"/>
       <c r="AJ34"/>
@@ -10060,8 +10204,9 @@
       <c r="BQ34"/>
       <c r="BR34"/>
       <c r="BS34"/>
-    </row>
-    <row r="35" spans="1:71" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT34"/>
+    </row>
+    <row r="35" spans="1:72" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>35</v>
       </c>
@@ -10154,8 +10299,11 @@
       <c r="AB35" s="6"/>
       <c r="AC35" s="6"/>
       <c r="AD35" s="6"/>
-      <c r="AE35" s="6"/>
-      <c r="AF35"/>
+      <c r="AE35" s="6" t="str">
+        <f>IF(V35&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF35" s="6"/>
       <c r="AG35"/>
       <c r="AH35"/>
       <c r="AI35"/>
@@ -10195,8 +10343,9 @@
       <c r="BQ35"/>
       <c r="BR35"/>
       <c r="BS35"/>
-    </row>
-    <row r="36" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT35"/>
+    </row>
+    <row r="36" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>30</v>
       </c>
@@ -10287,9 +10436,13 @@
       <c r="AB36" s="6"/>
       <c r="AC36" s="6"/>
       <c r="AD36" s="6"/>
-      <c r="AE36" s="6"/>
-    </row>
-    <row r="37" spans="1:71" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE36" s="6" t="str">
+        <f>IF(V36&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF36" s="6"/>
+    </row>
+    <row r="37" spans="1:72" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>29</v>
       </c>
@@ -10380,8 +10533,11 @@
       <c r="AB37" s="6"/>
       <c r="AC37" s="6"/>
       <c r="AD37" s="6"/>
-      <c r="AE37" s="6"/>
-      <c r="AF37"/>
+      <c r="AE37" s="6" t="str">
+        <f>IF(V37&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF37" s="6"/>
       <c r="AG37"/>
       <c r="AH37"/>
       <c r="AI37"/>
@@ -10421,8 +10577,9 @@
       <c r="BQ37"/>
       <c r="BR37"/>
       <c r="BS37"/>
-    </row>
-    <row r="38" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT37"/>
+    </row>
+    <row r="38" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>21</v>
       </c>
@@ -10513,11 +10670,14 @@
         <v>1</v>
       </c>
       <c r="AD38" s="5"/>
-      <c r="AE38" s="5"/>
-      <c r="AF38" s="2">
+      <c r="AE38" s="5">
+        <f>IF(V38&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG38"/>
+      <c r="AF38" s="5"/>
+      <c r="AG38" s="2">
+        <v>1</v>
+      </c>
       <c r="AH38"/>
       <c r="AI38"/>
       <c r="AJ38"/>
@@ -10556,8 +10716,9 @@
       <c r="BQ38"/>
       <c r="BR38"/>
       <c r="BS38"/>
-    </row>
-    <row r="39" spans="1:71" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT38"/>
+    </row>
+    <row r="39" spans="1:72" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>22</v>
       </c>
@@ -10648,8 +10809,11 @@
       <c r="AB39" s="6"/>
       <c r="AC39" s="6"/>
       <c r="AD39" s="6"/>
-      <c r="AE39" s="6"/>
-      <c r="AF39"/>
+      <c r="AE39" s="6" t="str">
+        <f>IF(V39&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF39" s="6"/>
       <c r="AG39"/>
       <c r="AH39"/>
       <c r="AI39"/>
@@ -10689,8 +10853,9 @@
       <c r="BQ39"/>
       <c r="BR39"/>
       <c r="BS39"/>
-    </row>
-    <row r="40" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT39"/>
+    </row>
+    <row r="40" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>121</v>
       </c>
@@ -10781,11 +10946,14 @@
       <c r="AD40" s="5">
         <v>1</v>
       </c>
-      <c r="AE40" s="5"/>
-      <c r="AF40" s="2">
+      <c r="AE40" s="5">
+        <f>IF(V40&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG40"/>
+      <c r="AF40" s="5"/>
+      <c r="AG40" s="2">
+        <v>1</v>
+      </c>
       <c r="AH40"/>
       <c r="AI40"/>
       <c r="AJ40"/>
@@ -10824,8 +10992,9 @@
       <c r="BQ40"/>
       <c r="BR40"/>
       <c r="BS40"/>
-    </row>
-    <row r="41" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT40"/>
+    </row>
+    <row r="41" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>118</v>
       </c>
@@ -10916,9 +11085,13 @@
       <c r="AB41" s="6"/>
       <c r="AC41" s="6"/>
       <c r="AD41" s="6"/>
-      <c r="AE41" s="6"/>
-    </row>
-    <row r="42" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE41" s="6" t="str">
+        <f>IF(V41&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF41" s="6"/>
+    </row>
+    <row r="42" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>117</v>
       </c>
@@ -11009,9 +11182,13 @@
       <c r="AB42" s="6"/>
       <c r="AC42" s="6"/>
       <c r="AD42" s="6"/>
-      <c r="AE42" s="6"/>
-    </row>
-    <row r="43" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE42" s="6" t="str">
+        <f>IF(V42&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF42" s="6"/>
+    </row>
+    <row r="43" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>83</v>
       </c>
@@ -11102,9 +11279,13 @@
       <c r="AB43" s="6"/>
       <c r="AC43" s="6"/>
       <c r="AD43" s="6"/>
-      <c r="AE43" s="6"/>
-    </row>
-    <row r="44" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE43" s="6" t="str">
+        <f>IF(V43&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF43" s="6"/>
+    </row>
+    <row r="44" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>102</v>
       </c>
@@ -11197,11 +11378,14 @@
       <c r="AD44" s="5">
         <v>1</v>
       </c>
-      <c r="AE44" s="5"/>
-      <c r="AF44" s="2">
+      <c r="AE44" s="5" t="str">
+        <f>IF(V44&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF44" s="5"/>
+      <c r="AG44" s="2">
         <v>1</v>
       </c>
-      <c r="AG44"/>
       <c r="AH44"/>
       <c r="AI44"/>
       <c r="AJ44"/>
@@ -11240,8 +11424,9 @@
       <c r="BQ44"/>
       <c r="BR44"/>
       <c r="BS44"/>
-    </row>
-    <row r="45" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT44"/>
+    </row>
+    <row r="45" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>70</v>
       </c>
@@ -11330,9 +11515,13 @@
       <c r="AB45" s="6"/>
       <c r="AC45" s="6"/>
       <c r="AD45" s="6"/>
-      <c r="AE45" s="6"/>
-    </row>
-    <row r="46" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE45" s="6" t="str">
+        <f>IF(V45&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF45" s="6"/>
+    </row>
+    <row r="46" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>84</v>
       </c>
@@ -11421,9 +11610,13 @@
       <c r="AB46" s="6"/>
       <c r="AC46" s="6"/>
       <c r="AD46" s="6"/>
-      <c r="AE46" s="6"/>
-    </row>
-    <row r="47" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE46" s="6" t="str">
+        <f>IF(V46&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF46" s="6"/>
+    </row>
+    <row r="47" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>73</v>
       </c>
@@ -11514,9 +11707,13 @@
       <c r="AB47" s="6"/>
       <c r="AC47" s="6"/>
       <c r="AD47" s="6"/>
-      <c r="AE47" s="6"/>
-    </row>
-    <row r="48" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE47" s="6" t="str">
+        <f>IF(V47&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF47" s="6"/>
+    </row>
+    <row r="48" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>74</v>
       </c>
@@ -11607,9 +11804,13 @@
       <c r="AB48" s="6"/>
       <c r="AC48" s="6"/>
       <c r="AD48" s="6"/>
-      <c r="AE48" s="6"/>
-    </row>
-    <row r="49" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE48" s="6" t="str">
+        <f>IF(V48&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF48" s="6"/>
+    </row>
+    <row r="49" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>103</v>
       </c>
@@ -11698,9 +11899,13 @@
       <c r="AB49" s="6"/>
       <c r="AC49" s="6"/>
       <c r="AD49" s="6"/>
-      <c r="AE49" s="6"/>
-    </row>
-    <row r="50" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE49" s="6" t="str">
+        <f>IF(V49&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF49" s="6"/>
+    </row>
+    <row r="50" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>68</v>
       </c>
@@ -11791,9 +11996,13 @@
       <c r="AB50" s="6"/>
       <c r="AC50" s="6"/>
       <c r="AD50" s="6"/>
-      <c r="AE50" s="6"/>
-    </row>
-    <row r="51" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE50" s="6" t="str">
+        <f>IF(V50&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF50" s="6"/>
+    </row>
+    <row r="51" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>69</v>
       </c>
@@ -11884,9 +12093,13 @@
       <c r="AB51" s="6"/>
       <c r="AC51" s="6"/>
       <c r="AD51" s="6"/>
-      <c r="AE51" s="6"/>
-    </row>
-    <row r="52" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE51" s="6" t="str">
+        <f>IF(V51&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF51" s="6"/>
+    </row>
+    <row r="52" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
         <v>100</v>
       </c>
@@ -11979,11 +12192,14 @@
       <c r="AD52" s="5">
         <v>1</v>
       </c>
-      <c r="AE52" s="5"/>
-      <c r="AF52" s="2">
+      <c r="AE52" s="5">
+        <f>IF(V52&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG52"/>
+      <c r="AF52" s="5"/>
+      <c r="AG52" s="2">
+        <v>1</v>
+      </c>
       <c r="AH52"/>
       <c r="AI52"/>
       <c r="AJ52"/>
@@ -12022,8 +12238,9 @@
       <c r="BQ52"/>
       <c r="BR52"/>
       <c r="BS52"/>
-    </row>
-    <row r="53" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT52"/>
+    </row>
+    <row r="53" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>99</v>
       </c>
@@ -12112,9 +12329,13 @@
       <c r="AB53" s="6"/>
       <c r="AC53" s="6"/>
       <c r="AD53" s="6"/>
-      <c r="AE53" s="6"/>
-    </row>
-    <row r="54" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE53" s="6" t="str">
+        <f>IF(V53&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF53" s="6"/>
+    </row>
+    <row r="54" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>87</v>
       </c>
@@ -12205,9 +12426,13 @@
       <c r="AB54" s="6"/>
       <c r="AC54" s="6"/>
       <c r="AD54" s="6"/>
-      <c r="AE54" s="6"/>
-    </row>
-    <row r="55" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE54" s="6" t="str">
+        <f>IF(V54&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF54" s="6"/>
+    </row>
+    <row r="55" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
         <v>76</v>
       </c>
@@ -12298,9 +12523,13 @@
       <c r="AB55" s="6"/>
       <c r="AC55" s="6"/>
       <c r="AD55" s="6"/>
-      <c r="AE55" s="6"/>
-    </row>
-    <row r="56" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE55" s="6" t="str">
+        <f>IF(V55&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF55" s="6"/>
+    </row>
+    <row r="56" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>93</v>
       </c>
@@ -12389,9 +12618,13 @@
       <c r="AB56" s="6"/>
       <c r="AC56" s="6"/>
       <c r="AD56" s="6"/>
-      <c r="AE56" s="6"/>
-    </row>
-    <row r="57" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE56" s="6" t="str">
+        <f>IF(V56&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF56" s="6"/>
+    </row>
+    <row r="57" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
         <v>65</v>
       </c>
@@ -12482,9 +12715,13 @@
       <c r="AB57" s="6"/>
       <c r="AC57" s="6"/>
       <c r="AD57" s="6"/>
-      <c r="AE57" s="6"/>
-    </row>
-    <row r="58" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE57" s="6" t="str">
+        <f>IF(V57&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF57" s="6"/>
+    </row>
+    <row r="58" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
         <v>66</v>
       </c>
@@ -12573,9 +12810,13 @@
       <c r="AB58" s="6"/>
       <c r="AC58" s="6"/>
       <c r="AD58" s="6"/>
-      <c r="AE58" s="6"/>
-    </row>
-    <row r="59" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE58" s="6">
+        <f>IF(V58&lt;5,1,"")</f>
+        <v>1</v>
+      </c>
+      <c r="AF58" s="6"/>
+    </row>
+    <row r="59" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5">
         <v>86</v>
       </c>
@@ -12668,11 +12909,14 @@
       <c r="AD59" s="5">
         <v>1</v>
       </c>
-      <c r="AE59" s="5"/>
-      <c r="AF59" s="2">
+      <c r="AE59" s="5" t="str">
+        <f>IF(V59&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF59" s="5"/>
+      <c r="AG59" s="2">
         <v>1</v>
       </c>
-      <c r="AG59"/>
       <c r="AH59"/>
       <c r="AI59"/>
       <c r="AJ59"/>
@@ -12711,8 +12955,9 @@
       <c r="BQ59"/>
       <c r="BR59"/>
       <c r="BS59"/>
-    </row>
-    <row r="60" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT59"/>
+    </row>
+    <row r="60" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
         <v>94</v>
       </c>
@@ -12805,11 +13050,14 @@
       <c r="AD60" s="5">
         <v>1</v>
       </c>
-      <c r="AE60" s="5"/>
-      <c r="AF60" s="2">
+      <c r="AE60" s="5" t="str">
+        <f>IF(V60&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF60" s="5"/>
+      <c r="AG60" s="2">
         <v>1</v>
       </c>
-      <c r="AG60"/>
       <c r="AH60"/>
       <c r="AI60"/>
       <c r="AJ60"/>
@@ -12848,8 +13096,9 @@
       <c r="BQ60"/>
       <c r="BR60"/>
       <c r="BS60"/>
-    </row>
-    <row r="61" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT60"/>
+    </row>
+    <row r="61" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
         <v>85</v>
       </c>
@@ -12938,9 +13187,13 @@
       <c r="AB61" s="6"/>
       <c r="AC61" s="6"/>
       <c r="AD61" s="6"/>
-      <c r="AE61" s="6"/>
-    </row>
-    <row r="62" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE61" s="6" t="str">
+        <f>IF(V61&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF61" s="6"/>
+    </row>
+    <row r="62" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
         <v>90</v>
       </c>
@@ -13029,9 +13282,13 @@
       <c r="AB62" s="6"/>
       <c r="AC62" s="6"/>
       <c r="AD62" s="6"/>
-      <c r="AE62" s="6"/>
-    </row>
-    <row r="63" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE62" s="6" t="str">
+        <f>IF(V62&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF62" s="6"/>
+    </row>
+    <row r="63" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>88</v>
       </c>
@@ -13120,9 +13377,13 @@
       <c r="AB63" s="6"/>
       <c r="AC63" s="6"/>
       <c r="AD63" s="6"/>
-      <c r="AE63" s="6"/>
-    </row>
-    <row r="64" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE63" s="6" t="str">
+        <f>IF(V63&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF63" s="6"/>
+    </row>
+    <row r="64" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>89</v>
       </c>
@@ -13213,9 +13474,13 @@
       <c r="AB64" s="6"/>
       <c r="AC64" s="6"/>
       <c r="AD64" s="6"/>
-      <c r="AE64" s="6"/>
-    </row>
-    <row r="65" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE64" s="6" t="str">
+        <f>IF(V64&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF64" s="6"/>
+    </row>
+    <row r="65" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>91</v>
       </c>
@@ -13306,9 +13571,13 @@
       <c r="AB65" s="6"/>
       <c r="AC65" s="6"/>
       <c r="AD65" s="6"/>
-      <c r="AE65" s="6"/>
-    </row>
-    <row r="66" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE65" s="6" t="str">
+        <f>IF(V65&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF65" s="6"/>
+    </row>
+    <row r="66" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
         <v>78</v>
       </c>
@@ -13399,9 +13668,13 @@
       <c r="AB66" s="6"/>
       <c r="AC66" s="6"/>
       <c r="AD66" s="6"/>
-      <c r="AE66" s="6"/>
-    </row>
-    <row r="67" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE66" s="6" t="str">
+        <f>IF(V66&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF66" s="6"/>
+    </row>
+    <row r="67" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5">
         <v>75</v>
       </c>
@@ -13487,11 +13760,14 @@
       </c>
       <c r="AC67" s="5"/>
       <c r="AD67" s="5"/>
-      <c r="AE67" s="5"/>
-      <c r="AF67" s="2">
+      <c r="AE67" s="5">
+        <f>IF(V67&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG67"/>
+      <c r="AF67" s="5"/>
+      <c r="AG67" s="2">
+        <v>1</v>
+      </c>
       <c r="AH67"/>
       <c r="AI67"/>
       <c r="AJ67"/>
@@ -13530,8 +13806,9 @@
       <c r="BQ67"/>
       <c r="BR67"/>
       <c r="BS67"/>
-    </row>
-    <row r="68" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT67"/>
+    </row>
+    <row r="68" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
         <v>79</v>
       </c>
@@ -13620,9 +13897,13 @@
       <c r="AB68" s="6"/>
       <c r="AC68" s="6"/>
       <c r="AD68" s="6"/>
-      <c r="AE68" s="6"/>
-    </row>
-    <row r="69" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE68" s="6" t="str">
+        <f>IF(V68&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF68" s="6"/>
+    </row>
+    <row r="69" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A69" s="6">
         <v>71</v>
       </c>
@@ -13713,9 +13994,13 @@
       <c r="AB69" s="6"/>
       <c r="AC69" s="6"/>
       <c r="AD69" s="6"/>
-      <c r="AE69" s="6"/>
-    </row>
-    <row r="70" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE69" s="6" t="str">
+        <f>IF(V69&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF69" s="6"/>
+    </row>
+    <row r="70" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>67</v>
       </c>
@@ -13806,9 +14091,13 @@
       <c r="AB70" s="6"/>
       <c r="AC70" s="6"/>
       <c r="AD70" s="6"/>
-      <c r="AE70" s="6"/>
-    </row>
-    <row r="71" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE70" s="6" t="str">
+        <f>IF(V70&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF70" s="6"/>
+    </row>
+    <row r="71" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
         <v>92</v>
       </c>
@@ -13897,9 +14186,13 @@
       <c r="AB71" s="6"/>
       <c r="AC71" s="6"/>
       <c r="AD71" s="6"/>
-      <c r="AE71" s="6"/>
-    </row>
-    <row r="72" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE71" s="6" t="str">
+        <f>IF(V71&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF71" s="6"/>
+    </row>
+    <row r="72" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>77</v>
       </c>
@@ -13990,9 +14283,13 @@
       <c r="AB72" s="6"/>
       <c r="AC72" s="6"/>
       <c r="AD72" s="6"/>
-      <c r="AE72" s="6"/>
-    </row>
-    <row r="73" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE72" s="6" t="str">
+        <f>IF(V72&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF72" s="6"/>
+    </row>
+    <row r="73" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A73" s="6">
         <v>96</v>
       </c>
@@ -14083,9 +14380,13 @@
       <c r="AB73" s="6"/>
       <c r="AC73" s="6"/>
       <c r="AD73" s="6"/>
-      <c r="AE73" s="6"/>
-    </row>
-    <row r="74" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE73" s="6" t="str">
+        <f>IF(V73&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF73" s="6"/>
+    </row>
+    <row r="74" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A74" s="6">
         <v>97</v>
       </c>
@@ -14176,9 +14477,13 @@
       <c r="AB74" s="6"/>
       <c r="AC74" s="6"/>
       <c r="AD74" s="6"/>
-      <c r="AE74" s="6"/>
-    </row>
-    <row r="75" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE74" s="6" t="str">
+        <f>IF(V74&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF74" s="6"/>
+    </row>
+    <row r="75" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A75" s="6">
         <v>98</v>
       </c>
@@ -14269,9 +14574,13 @@
       <c r="AB75" s="6"/>
       <c r="AC75" s="6"/>
       <c r="AD75" s="6"/>
-      <c r="AE75" s="6"/>
-    </row>
-    <row r="76" spans="1:71" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE75" s="6" t="str">
+        <f>IF(V75&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF75" s="6"/>
+    </row>
+    <row r="76" spans="1:72" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
         <v>95</v>
       </c>
@@ -14362,8 +14671,11 @@
       <c r="AB76" s="6"/>
       <c r="AC76" s="6"/>
       <c r="AD76" s="6"/>
-      <c r="AE76" s="6"/>
-      <c r="AF76"/>
+      <c r="AE76" s="6" t="str">
+        <f>IF(V76&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF76" s="6"/>
       <c r="AG76"/>
       <c r="AH76"/>
       <c r="AI76"/>
@@ -14403,8 +14715,9 @@
       <c r="BQ76"/>
       <c r="BR76"/>
       <c r="BS76"/>
-    </row>
-    <row r="77" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT76"/>
+    </row>
+    <row r="77" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A77" s="6">
         <v>82</v>
       </c>
@@ -14493,9 +14806,13 @@
       <c r="AB77" s="6"/>
       <c r="AC77" s="6"/>
       <c r="AD77" s="6"/>
-      <c r="AE77" s="6"/>
-    </row>
-    <row r="78" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE77" s="6" t="str">
+        <f>IF(V77&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF77" s="6"/>
+    </row>
+    <row r="78" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A78" s="6">
         <v>81</v>
       </c>
@@ -14586,9 +14903,13 @@
       <c r="AB78" s="6"/>
       <c r="AC78" s="6"/>
       <c r="AD78" s="6"/>
-      <c r="AE78" s="6"/>
-    </row>
-    <row r="79" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE78" s="6" t="str">
+        <f>IF(V78&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF78" s="6"/>
+    </row>
+    <row r="79" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A79" s="6">
         <v>80</v>
       </c>
@@ -14679,9 +15000,13 @@
       <c r="AB79" s="6"/>
       <c r="AC79" s="6"/>
       <c r="AD79" s="6"/>
-      <c r="AE79" s="6"/>
-    </row>
-    <row r="80" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE79" s="6" t="str">
+        <f>IF(V79&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF79" s="6"/>
+    </row>
+    <row r="80" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="5">
         <v>101</v>
       </c>
@@ -14774,11 +15099,14 @@
       <c r="AD80" s="5">
         <v>1</v>
       </c>
-      <c r="AE80" s="5"/>
-      <c r="AF80" s="2">
+      <c r="AE80" s="5" t="str">
+        <f>IF(V80&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF80" s="5"/>
+      <c r="AG80" s="2">
         <v>1</v>
       </c>
-      <c r="AG80"/>
       <c r="AH80"/>
       <c r="AI80"/>
       <c r="AJ80"/>
@@ -14817,8 +15145,9 @@
       <c r="BQ80"/>
       <c r="BR80"/>
       <c r="BS80"/>
-    </row>
-    <row r="81" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT80"/>
+    </row>
+    <row r="81" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A81" s="6">
         <v>72</v>
       </c>
@@ -14909,9 +15238,13 @@
       <c r="AB81" s="6"/>
       <c r="AC81" s="6"/>
       <c r="AD81" s="6"/>
-      <c r="AE81" s="6"/>
-    </row>
-    <row r="82" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE81" s="6" t="str">
+        <f>IF(V81&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF81" s="6"/>
+    </row>
+    <row r="82" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A82" s="6">
         <v>12</v>
       </c>
@@ -15002,9 +15335,13 @@
       <c r="AB82" s="6"/>
       <c r="AC82" s="6"/>
       <c r="AD82" s="6"/>
-      <c r="AE82" s="6"/>
-    </row>
-    <row r="83" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE82" s="6" t="str">
+        <f>IF(V82&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF82" s="6"/>
+    </row>
+    <row r="83" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="5">
         <v>11</v>
       </c>
@@ -15095,11 +15432,14 @@
       </c>
       <c r="AC83" s="5"/>
       <c r="AD83" s="5"/>
-      <c r="AE83" s="5"/>
-      <c r="AF83" s="2">
+      <c r="AE83" s="5">
+        <f>IF(V83&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG83"/>
+      <c r="AF83" s="5"/>
+      <c r="AG83" s="2">
+        <v>1</v>
+      </c>
       <c r="AH83"/>
       <c r="AI83"/>
       <c r="AJ83"/>
@@ -15138,8 +15478,9 @@
       <c r="BQ83"/>
       <c r="BR83"/>
       <c r="BS83"/>
-    </row>
-    <row r="84" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT83"/>
+    </row>
+    <row r="84" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="5">
         <v>104</v>
       </c>
@@ -15225,13 +15566,16 @@
       <c r="AB84" s="5"/>
       <c r="AC84" s="5"/>
       <c r="AD84" s="5"/>
-      <c r="AE84" s="5">
+      <c r="AE84" s="5" t="str">
+        <f>IF(V84&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF84" s="5">
         <v>1</v>
       </c>
-      <c r="AF84" s="2">
+      <c r="AG84" s="2">
         <v>1</v>
       </c>
-      <c r="AG84"/>
       <c r="AH84"/>
       <c r="AI84"/>
       <c r="AJ84"/>
@@ -15270,8 +15614,9 @@
       <c r="BQ84"/>
       <c r="BR84"/>
       <c r="BS84"/>
-    </row>
-    <row r="85" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT84"/>
+    </row>
+    <row r="85" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A85" s="6">
         <v>105</v>
       </c>
@@ -15362,9 +15707,13 @@
       <c r="AB85" s="6"/>
       <c r="AC85" s="6"/>
       <c r="AD85" s="6"/>
-      <c r="AE85" s="6"/>
-    </row>
-    <row r="86" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE85" s="6" t="str">
+        <f>IF(V85&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF85" s="6"/>
+    </row>
+    <row r="86" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A86" s="6">
         <v>106</v>
       </c>
@@ -15455,9 +15804,13 @@
       <c r="AB86" s="6"/>
       <c r="AC86" s="6"/>
       <c r="AD86" s="6"/>
-      <c r="AE86" s="6"/>
-    </row>
-    <row r="87" spans="1:71" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE86" s="6" t="str">
+        <f>IF(V86&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF86" s="6"/>
+    </row>
+    <row r="87" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="6">
         <v>107</v>
       </c>
@@ -15548,8 +15901,11 @@
       <c r="AB87" s="6"/>
       <c r="AC87" s="6"/>
       <c r="AD87" s="6"/>
-      <c r="AE87" s="6"/>
-      <c r="AF87"/>
+      <c r="AE87" s="6" t="str">
+        <f>IF(V87&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF87" s="6"/>
       <c r="AG87"/>
       <c r="AH87"/>
       <c r="AI87"/>
@@ -15589,8 +15945,9 @@
       <c r="BQ87"/>
       <c r="BR87"/>
       <c r="BS87"/>
-    </row>
-    <row r="88" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT87"/>
+    </row>
+    <row r="88" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A88" s="6">
         <v>108</v>
       </c>
@@ -15681,9 +16038,13 @@
       <c r="AB88" s="6"/>
       <c r="AC88" s="6"/>
       <c r="AD88" s="6"/>
-      <c r="AE88" s="6"/>
-    </row>
-    <row r="89" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE88" s="6" t="str">
+        <f>IF(V88&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF88" s="6"/>
+    </row>
+    <row r="89" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A89" s="6">
         <v>119</v>
       </c>
@@ -15772,9 +16133,13 @@
       <c r="AB89" s="6"/>
       <c r="AC89" s="6"/>
       <c r="AD89" s="6"/>
-      <c r="AE89" s="6"/>
-    </row>
-    <row r="90" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE89" s="6" t="str">
+        <f>IF(V89&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF89" s="6"/>
+    </row>
+    <row r="90" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="5">
         <v>120</v>
       </c>
@@ -15867,11 +16232,14 @@
       <c r="AD90" s="5">
         <v>1</v>
       </c>
-      <c r="AE90" s="5"/>
-      <c r="AF90" s="2">
+      <c r="AE90" s="5">
+        <f>IF(V90&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG90"/>
+      <c r="AF90" s="5"/>
+      <c r="AG90" s="2">
+        <v>1</v>
+      </c>
       <c r="AH90"/>
       <c r="AI90"/>
       <c r="AJ90"/>
@@ -15910,8 +16278,9 @@
       <c r="BQ90"/>
       <c r="BR90"/>
       <c r="BS90"/>
-    </row>
-    <row r="91" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT90"/>
+    </row>
+    <row r="91" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A91" s="6">
         <v>109</v>
       </c>
@@ -16000,9 +16369,13 @@
       <c r="AB91" s="6"/>
       <c r="AC91" s="6"/>
       <c r="AD91" s="6"/>
-      <c r="AE91" s="6"/>
-    </row>
-    <row r="92" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE91" s="6" t="str">
+        <f>IF(V91&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF91" s="6"/>
+    </row>
+    <row r="92" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A92" s="6">
         <v>54</v>
       </c>
@@ -16091,9 +16464,13 @@
       <c r="AB92" s="6"/>
       <c r="AC92" s="6"/>
       <c r="AD92" s="6"/>
-      <c r="AE92" s="6"/>
-    </row>
-    <row r="93" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE92" s="6" t="str">
+        <f>IF(V92&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF92" s="6"/>
+    </row>
+    <row r="93" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A93" s="6">
         <v>53</v>
       </c>
@@ -16184,9 +16561,13 @@
       <c r="AB93" s="6"/>
       <c r="AC93" s="6"/>
       <c r="AD93" s="6"/>
-      <c r="AE93" s="6"/>
-    </row>
-    <row r="94" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE93" s="6" t="str">
+        <f>IF(V93&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF93" s="6"/>
+    </row>
+    <row r="94" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A94" s="6">
         <v>52</v>
       </c>
@@ -16275,9 +16656,13 @@
       <c r="AB94" s="6"/>
       <c r="AC94" s="6"/>
       <c r="AD94" s="6"/>
-      <c r="AE94" s="6"/>
-    </row>
-    <row r="95" spans="1:71" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE94" s="6" t="str">
+        <f>IF(V94&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF94" s="6"/>
+    </row>
+    <row r="95" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="6">
         <v>57</v>
       </c>
@@ -16368,8 +16753,11 @@
       <c r="AB95" s="6"/>
       <c r="AC95" s="6"/>
       <c r="AD95" s="6"/>
-      <c r="AE95" s="6"/>
-      <c r="AF95"/>
+      <c r="AE95" s="6" t="str">
+        <f>IF(V95&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF95" s="6"/>
       <c r="AG95"/>
       <c r="AH95"/>
       <c r="AI95"/>
@@ -16409,8 +16797,9 @@
       <c r="BQ95"/>
       <c r="BR95"/>
       <c r="BS95"/>
-    </row>
-    <row r="96" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT95"/>
+    </row>
+    <row r="96" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A96" s="6">
         <v>55</v>
       </c>
@@ -16499,9 +16888,13 @@
       <c r="AB96" s="6"/>
       <c r="AC96" s="6"/>
       <c r="AD96" s="6"/>
-      <c r="AE96" s="6"/>
-    </row>
-    <row r="97" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE96" s="6" t="str">
+        <f>IF(V96&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF96" s="6"/>
+    </row>
+    <row r="97" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A97" s="6">
         <v>56</v>
       </c>
@@ -16590,9 +16983,13 @@
       <c r="AB97" s="6"/>
       <c r="AC97" s="6"/>
       <c r="AD97" s="6"/>
-      <c r="AE97" s="6"/>
-    </row>
-    <row r="98" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE97" s="6" t="str">
+        <f>IF(V97&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF97" s="6"/>
+    </row>
+    <row r="98" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="5">
         <v>58</v>
       </c>
@@ -16685,11 +17082,14 @@
         <v>1</v>
       </c>
       <c r="AD98" s="5"/>
-      <c r="AE98" s="5"/>
-      <c r="AF98" s="2">
+      <c r="AE98" s="5" t="str">
+        <f>IF(V98&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF98" s="5"/>
+      <c r="AG98" s="2">
         <v>1</v>
       </c>
-      <c r="AG98"/>
       <c r="AH98"/>
       <c r="AI98"/>
       <c r="AJ98"/>
@@ -16728,8 +17128,9 @@
       <c r="BQ98"/>
       <c r="BR98"/>
       <c r="BS98"/>
-    </row>
-    <row r="99" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT98"/>
+    </row>
+    <row r="99" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A99" s="6">
         <v>61</v>
       </c>
@@ -16818,9 +17219,13 @@
       <c r="AB99" s="6"/>
       <c r="AC99" s="6"/>
       <c r="AD99" s="6"/>
-      <c r="AE99" s="6"/>
-    </row>
-    <row r="100" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE99" s="6" t="str">
+        <f>IF(V99&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF99" s="6"/>
+    </row>
+    <row r="100" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A100" s="6">
         <v>63</v>
       </c>
@@ -16911,9 +17316,13 @@
       <c r="AB100" s="6"/>
       <c r="AC100" s="6"/>
       <c r="AD100" s="6"/>
-      <c r="AE100" s="6"/>
-    </row>
-    <row r="101" spans="1:71" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE100" s="6" t="str">
+        <f>IF(V100&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF100" s="6"/>
+    </row>
+    <row r="101" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="6">
         <v>62</v>
       </c>
@@ -17004,8 +17413,11 @@
       <c r="AB101" s="6"/>
       <c r="AC101" s="6"/>
       <c r="AD101" s="6"/>
-      <c r="AE101" s="6"/>
-      <c r="AF101"/>
+      <c r="AE101" s="6" t="str">
+        <f>IF(V101&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF101" s="6"/>
       <c r="AG101"/>
       <c r="AH101"/>
       <c r="AI101"/>
@@ -17045,8 +17457,9 @@
       <c r="BQ101"/>
       <c r="BR101"/>
       <c r="BS101"/>
-    </row>
-    <row r="102" spans="1:71" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT101"/>
+    </row>
+    <row r="102" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="6">
         <v>64</v>
       </c>
@@ -17137,8 +17550,11 @@
       <c r="AB102" s="6"/>
       <c r="AC102" s="6"/>
       <c r="AD102" s="6"/>
-      <c r="AE102" s="6"/>
-      <c r="AF102"/>
+      <c r="AE102" s="6" t="str">
+        <f>IF(V102&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF102" s="6"/>
       <c r="AG102"/>
       <c r="AH102"/>
       <c r="AI102"/>
@@ -17178,8 +17594,9 @@
       <c r="BQ102"/>
       <c r="BR102"/>
       <c r="BS102"/>
-    </row>
-    <row r="103" spans="1:71" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT102"/>
+    </row>
+    <row r="103" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="6">
         <v>60</v>
       </c>
@@ -17270,8 +17687,11 @@
       <c r="AB103" s="6"/>
       <c r="AC103" s="6"/>
       <c r="AD103" s="6"/>
-      <c r="AE103" s="6"/>
-      <c r="AF103"/>
+      <c r="AE103" s="6" t="str">
+        <f>IF(V103&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF103" s="6"/>
       <c r="AG103"/>
       <c r="AH103"/>
       <c r="AI103"/>
@@ -17311,8 +17731,9 @@
       <c r="BQ103"/>
       <c r="BR103"/>
       <c r="BS103"/>
-    </row>
-    <row r="104" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT103"/>
+    </row>
+    <row r="104" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A104" s="6">
         <v>59</v>
       </c>
@@ -17403,9 +17824,13 @@
       <c r="AB104" s="6"/>
       <c r="AC104" s="6"/>
       <c r="AD104" s="6"/>
-      <c r="AE104" s="6"/>
-    </row>
-    <row r="105" spans="1:71" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE104" s="6" t="str">
+        <f>IF(V104&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF104" s="6"/>
+    </row>
+    <row r="105" spans="1:72" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="6">
         <v>218</v>
       </c>
@@ -17494,8 +17919,11 @@
       <c r="AB105" s="6"/>
       <c r="AC105" s="6"/>
       <c r="AD105" s="6"/>
-      <c r="AE105" s="6"/>
-      <c r="AF105"/>
+      <c r="AE105" s="6" t="str">
+        <f>IF(V105&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF105" s="6"/>
       <c r="AG105"/>
       <c r="AH105"/>
       <c r="AI105"/>
@@ -17535,8 +17963,9 @@
       <c r="BQ105"/>
       <c r="BR105"/>
       <c r="BS105"/>
-    </row>
-    <row r="106" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT105"/>
+    </row>
+    <row r="106" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A106" s="6">
         <v>168</v>
       </c>
@@ -17625,9 +18054,13 @@
       <c r="AB106" s="6"/>
       <c r="AC106" s="6"/>
       <c r="AD106" s="6"/>
-      <c r="AE106" s="6"/>
-    </row>
-    <row r="107" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE106" s="6" t="str">
+        <f>IF(V106&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF106" s="6"/>
+    </row>
+    <row r="107" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="5">
         <v>165</v>
       </c>
@@ -17718,11 +18151,14 @@
       <c r="AD107" s="5">
         <v>1</v>
       </c>
-      <c r="AE107" s="5"/>
-      <c r="AF107" s="2">
+      <c r="AE107" s="5">
+        <f>IF(V107&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG107"/>
+      <c r="AF107" s="5"/>
+      <c r="AG107" s="2">
+        <v>1</v>
+      </c>
       <c r="AH107"/>
       <c r="AI107"/>
       <c r="AJ107"/>
@@ -17761,8 +18197,9 @@
       <c r="BQ107"/>
       <c r="BR107"/>
       <c r="BS107"/>
-    </row>
-    <row r="108" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT107"/>
+    </row>
+    <row r="108" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A108" s="6">
         <v>166</v>
       </c>
@@ -17853,9 +18290,13 @@
       <c r="AB108" s="6"/>
       <c r="AC108" s="6"/>
       <c r="AD108" s="6"/>
-      <c r="AE108" s="6"/>
-    </row>
-    <row r="109" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE108" s="6" t="str">
+        <f>IF(V108&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF108" s="6"/>
+    </row>
+    <row r="109" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A109" s="6">
         <v>164</v>
       </c>
@@ -17946,9 +18387,13 @@
       <c r="AB109" s="6"/>
       <c r="AC109" s="6"/>
       <c r="AD109" s="6"/>
-      <c r="AE109" s="6"/>
-    </row>
-    <row r="110" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE109" s="6" t="str">
+        <f>IF(V109&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF109" s="6"/>
+    </row>
+    <row r="110" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A110" s="6">
         <v>167</v>
       </c>
@@ -18039,9 +18484,13 @@
       <c r="AB110" s="6"/>
       <c r="AC110" s="6"/>
       <c r="AD110" s="6"/>
-      <c r="AE110" s="6"/>
-    </row>
-    <row r="111" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE110" s="6" t="str">
+        <f>IF(V110&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF110" s="6"/>
+    </row>
+    <row r="111" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A111" s="6">
         <v>186</v>
       </c>
@@ -18132,9 +18581,13 @@
       <c r="AB111" s="6"/>
       <c r="AC111" s="6"/>
       <c r="AD111" s="6"/>
-      <c r="AE111" s="6"/>
-    </row>
-    <row r="112" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE111" s="6" t="str">
+        <f>IF(V111&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF111" s="6"/>
+    </row>
+    <row r="112" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A112" s="6">
         <v>130</v>
       </c>
@@ -18225,9 +18678,13 @@
       <c r="AB112" s="6"/>
       <c r="AC112" s="6"/>
       <c r="AD112" s="6"/>
-      <c r="AE112" s="6"/>
-    </row>
-    <row r="113" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE112" s="6" t="str">
+        <f>IF(V112&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF112" s="6"/>
+    </row>
+    <row r="113" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A113" s="6">
         <v>134</v>
       </c>
@@ -18316,9 +18773,13 @@
       <c r="AB113" s="6"/>
       <c r="AC113" s="6"/>
       <c r="AD113" s="6"/>
-      <c r="AE113" s="6"/>
-    </row>
-    <row r="114" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE113" s="6" t="str">
+        <f>IF(V113&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF113" s="6"/>
+    </row>
+    <row r="114" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A114" s="6">
         <v>137</v>
       </c>
@@ -18407,9 +18868,13 @@
       <c r="AB114" s="6"/>
       <c r="AC114" s="6"/>
       <c r="AD114" s="6"/>
-      <c r="AE114" s="6"/>
-    </row>
-    <row r="115" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE114" s="6" t="str">
+        <f>IF(V114&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF114" s="6"/>
+    </row>
+    <row r="115" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A115" s="6">
         <v>136</v>
       </c>
@@ -18500,9 +18965,13 @@
       <c r="AB115" s="6"/>
       <c r="AC115" s="6"/>
       <c r="AD115" s="6"/>
-      <c r="AE115" s="6"/>
-    </row>
-    <row r="116" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE115" s="6" t="str">
+        <f>IF(V115&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF115" s="6"/>
+    </row>
+    <row r="116" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A116" s="6">
         <v>135</v>
       </c>
@@ -18593,9 +19062,13 @@
       <c r="AB116" s="6"/>
       <c r="AC116" s="6"/>
       <c r="AD116" s="6"/>
-      <c r="AE116" s="6"/>
-    </row>
-    <row r="117" spans="1:71" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE116" s="6" t="str">
+        <f>IF(V116&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF116" s="6"/>
+    </row>
+    <row r="117" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="6">
         <v>215</v>
       </c>
@@ -18686,8 +19159,11 @@
       <c r="AB117" s="6"/>
       <c r="AC117" s="6"/>
       <c r="AD117" s="6"/>
-      <c r="AE117" s="6"/>
-      <c r="AF117"/>
+      <c r="AE117" s="6" t="str">
+        <f>IF(V117&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF117" s="6"/>
       <c r="AG117"/>
       <c r="AH117"/>
       <c r="AI117"/>
@@ -18727,8 +19203,9 @@
       <c r="BQ117"/>
       <c r="BR117"/>
       <c r="BS117"/>
-    </row>
-    <row r="118" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT117"/>
+    </row>
+    <row r="118" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A118" s="6">
         <v>222</v>
       </c>
@@ -18817,9 +19294,13 @@
       <c r="AB118" s="6"/>
       <c r="AC118" s="6"/>
       <c r="AD118" s="6"/>
-      <c r="AE118" s="6"/>
-    </row>
-    <row r="119" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE118" s="6" t="str">
+        <f>IF(V118&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF118" s="6"/>
+    </row>
+    <row r="119" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A119" s="6">
         <v>195</v>
       </c>
@@ -18910,9 +19391,13 @@
       <c r="AB119" s="6"/>
       <c r="AC119" s="6"/>
       <c r="AD119" s="6"/>
-      <c r="AE119" s="6"/>
-    </row>
-    <row r="120" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE119" s="6" t="str">
+        <f>IF(V119&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF119" s="6"/>
+    </row>
+    <row r="120" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A120" s="6">
         <v>194</v>
       </c>
@@ -19003,9 +19488,13 @@
       <c r="AB120" s="6"/>
       <c r="AC120" s="6"/>
       <c r="AD120" s="6"/>
-      <c r="AE120" s="6"/>
-    </row>
-    <row r="121" spans="1:71" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE120" s="6" t="str">
+        <f>IF(V120&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF120" s="6"/>
+    </row>
+    <row r="121" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="6">
         <v>214</v>
       </c>
@@ -19096,8 +19585,11 @@
       <c r="AB121" s="6"/>
       <c r="AC121" s="6"/>
       <c r="AD121" s="6"/>
-      <c r="AE121" s="6"/>
-      <c r="AF121"/>
+      <c r="AE121" s="6" t="str">
+        <f>IF(V121&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF121" s="6"/>
       <c r="AG121"/>
       <c r="AH121"/>
       <c r="AI121"/>
@@ -19137,8 +19629,9 @@
       <c r="BQ121"/>
       <c r="BR121"/>
       <c r="BS121"/>
-    </row>
-    <row r="122" spans="1:71" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT121"/>
+    </row>
+    <row r="122" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="6">
         <v>143</v>
       </c>
@@ -19227,8 +19720,11 @@
       <c r="AB122" s="6"/>
       <c r="AC122" s="6"/>
       <c r="AD122" s="6"/>
-      <c r="AE122" s="6"/>
-      <c r="AF122"/>
+      <c r="AE122" s="6" t="str">
+        <f>IF(V122&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF122" s="6"/>
       <c r="AG122"/>
       <c r="AH122"/>
       <c r="AI122"/>
@@ -19268,8 +19764,9 @@
       <c r="BQ122"/>
       <c r="BR122"/>
       <c r="BS122"/>
-    </row>
-    <row r="123" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT122"/>
+    </row>
+    <row r="123" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A123" s="6">
         <v>224</v>
       </c>
@@ -19360,9 +19857,13 @@
       <c r="AB123" s="6"/>
       <c r="AC123" s="6"/>
       <c r="AD123" s="6"/>
-      <c r="AE123" s="6"/>
-    </row>
-    <row r="124" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE123" s="6" t="str">
+        <f>IF(V123&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF123" s="6"/>
+    </row>
+    <row r="124" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A124" s="6">
         <v>203</v>
       </c>
@@ -19453,9 +19954,13 @@
       <c r="AB124" s="6"/>
       <c r="AC124" s="6"/>
       <c r="AD124" s="6"/>
-      <c r="AE124" s="6"/>
-    </row>
-    <row r="125" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE124" s="6" t="str">
+        <f>IF(V124&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF124" s="6"/>
+    </row>
+    <row r="125" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A125" s="6">
         <v>207</v>
       </c>
@@ -19546,9 +20051,13 @@
       <c r="AB125" s="6"/>
       <c r="AC125" s="6"/>
       <c r="AD125" s="6"/>
-      <c r="AE125" s="6"/>
-    </row>
-    <row r="126" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE125" s="6" t="str">
+        <f>IF(V125&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF125" s="6"/>
+    </row>
+    <row r="126" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A126" s="6">
         <v>206</v>
       </c>
@@ -19637,9 +20146,13 @@
       <c r="AB126" s="6"/>
       <c r="AC126" s="6"/>
       <c r="AD126" s="6"/>
-      <c r="AE126" s="6"/>
-    </row>
-    <row r="127" spans="1:71" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE126" s="6" t="str">
+        <f>IF(V126&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF126" s="6"/>
+    </row>
+    <row r="127" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="6">
         <v>205</v>
       </c>
@@ -19730,8 +20243,11 @@
       <c r="AB127" s="6"/>
       <c r="AC127" s="6"/>
       <c r="AD127" s="6"/>
-      <c r="AE127" s="6"/>
-      <c r="AF127"/>
+      <c r="AE127" s="6" t="str">
+        <f>IF(V127&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF127" s="6"/>
       <c r="AG127"/>
       <c r="AH127"/>
       <c r="AI127"/>
@@ -19771,8 +20287,9 @@
       <c r="BQ127"/>
       <c r="BR127"/>
       <c r="BS127"/>
-    </row>
-    <row r="128" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT127"/>
+    </row>
+    <row r="128" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A128" s="6">
         <v>204</v>
       </c>
@@ -19863,9 +20380,13 @@
       <c r="AB128" s="6"/>
       <c r="AC128" s="6"/>
       <c r="AD128" s="6"/>
-      <c r="AE128" s="6"/>
-    </row>
-    <row r="129" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE128" s="6" t="str">
+        <f>IF(V128&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF128" s="6"/>
+    </row>
+    <row r="129" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A129" s="6">
         <v>172</v>
       </c>
@@ -19954,9 +20475,13 @@
       <c r="AB129" s="6"/>
       <c r="AC129" s="6"/>
       <c r="AD129" s="6"/>
-      <c r="AE129" s="6"/>
-    </row>
-    <row r="130" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE129" s="6" t="str">
+        <f>IF(V129&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF129" s="6"/>
+    </row>
+    <row r="130" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A130" s="6">
         <v>171</v>
       </c>
@@ -20047,9 +20572,13 @@
       <c r="AB130" s="6"/>
       <c r="AC130" s="6"/>
       <c r="AD130" s="6"/>
-      <c r="AE130" s="6"/>
-    </row>
-    <row r="131" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE130" s="6" t="str">
+        <f>IF(V130&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF130" s="6"/>
+    </row>
+    <row r="131" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A131" s="6">
         <v>170</v>
       </c>
@@ -20138,9 +20667,13 @@
       <c r="AB131" s="6"/>
       <c r="AC131" s="6"/>
       <c r="AD131" s="6"/>
-      <c r="AE131" s="6"/>
-    </row>
-    <row r="132" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE131" s="6" t="str">
+        <f>IF(V131&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF131" s="6"/>
+    </row>
+    <row r="132" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A132" s="6">
         <v>191</v>
       </c>
@@ -20229,9 +20762,13 @@
       <c r="AB132" s="6"/>
       <c r="AC132" s="6"/>
       <c r="AD132" s="6"/>
-      <c r="AE132" s="6"/>
-    </row>
-    <row r="133" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE132" s="6" t="str">
+        <f>IF(V132&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF132" s="6"/>
+    </row>
+    <row r="133" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A133" s="6">
         <v>133</v>
       </c>
@@ -20322,9 +20859,13 @@
       <c r="AB133" s="6"/>
       <c r="AC133" s="6"/>
       <c r="AD133" s="6"/>
-      <c r="AE133" s="6"/>
-    </row>
-    <row r="134" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE133" s="6" t="str">
+        <f>IF(V133&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF133" s="6"/>
+    </row>
+    <row r="134" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A134" s="6">
         <v>228</v>
       </c>
@@ -20413,9 +20954,13 @@
       <c r="AB134" s="6"/>
       <c r="AC134" s="6"/>
       <c r="AD134" s="6"/>
-      <c r="AE134" s="6"/>
-    </row>
-    <row r="135" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE134" s="6" t="str">
+        <f>IF(V134&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF134" s="6"/>
+    </row>
+    <row r="135" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A135" s="6">
         <v>225</v>
       </c>
@@ -20504,9 +21049,13 @@
       <c r="AB135" s="6"/>
       <c r="AC135" s="6"/>
       <c r="AD135" s="6"/>
-      <c r="AE135" s="6"/>
-    </row>
-    <row r="136" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE135" s="6" t="str">
+        <f>IF(V135&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF135" s="6"/>
+    </row>
+    <row r="136" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="5">
         <v>226</v>
       </c>
@@ -20592,11 +21141,14 @@
       </c>
       <c r="AC136" s="5"/>
       <c r="AD136" s="5"/>
-      <c r="AE136" s="5"/>
-      <c r="AF136" s="2">
+      <c r="AE136" s="5">
+        <f>IF(V136&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG136"/>
+      <c r="AF136" s="5"/>
+      <c r="AG136" s="2">
+        <v>1</v>
+      </c>
       <c r="AH136"/>
       <c r="AI136"/>
       <c r="AJ136"/>
@@ -20635,8 +21187,9 @@
       <c r="BQ136"/>
       <c r="BR136"/>
       <c r="BS136"/>
-    </row>
-    <row r="137" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT136"/>
+    </row>
+    <row r="137" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A137" s="6">
         <v>227</v>
       </c>
@@ -20725,9 +21278,13 @@
       <c r="AB137" s="6"/>
       <c r="AC137" s="6"/>
       <c r="AD137" s="6"/>
-      <c r="AE137" s="6"/>
-    </row>
-    <row r="138" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE137" s="6" t="str">
+        <f>IF(V137&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF137" s="6"/>
+    </row>
+    <row r="138" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A138" s="6">
         <v>146</v>
       </c>
@@ -20818,9 +21375,13 @@
       <c r="AB138" s="6"/>
       <c r="AC138" s="6"/>
       <c r="AD138" s="6"/>
-      <c r="AE138" s="6"/>
-    </row>
-    <row r="139" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE138" s="6" t="str">
+        <f>IF(V138&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF138" s="6"/>
+    </row>
+    <row r="139" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="5">
         <v>183</v>
       </c>
@@ -20911,11 +21472,14 @@
       <c r="AD139" s="5">
         <v>1</v>
       </c>
-      <c r="AE139" s="5"/>
-      <c r="AF139" s="2">
+      <c r="AE139" s="5">
+        <f>IF(V139&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG139"/>
+      <c r="AF139" s="5"/>
+      <c r="AG139" s="2">
+        <v>1</v>
+      </c>
       <c r="AH139"/>
       <c r="AI139"/>
       <c r="AJ139"/>
@@ -20954,8 +21518,9 @@
       <c r="BQ139"/>
       <c r="BR139"/>
       <c r="BS139"/>
-    </row>
-    <row r="140" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT139"/>
+    </row>
+    <row r="140" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A140" s="6">
         <v>184</v>
       </c>
@@ -21044,9 +21609,13 @@
       <c r="AB140" s="6"/>
       <c r="AC140" s="6"/>
       <c r="AD140" s="6"/>
-      <c r="AE140" s="6"/>
-    </row>
-    <row r="141" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE140" s="6" t="str">
+        <f>IF(V140&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF140" s="6"/>
+    </row>
+    <row r="141" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A141" s="6">
         <v>182</v>
       </c>
@@ -21135,9 +21704,13 @@
       <c r="AB141" s="6"/>
       <c r="AC141" s="6"/>
       <c r="AD141" s="6"/>
-      <c r="AE141" s="6"/>
-    </row>
-    <row r="142" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE141" s="6" t="str">
+        <f>IF(V141&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF141" s="6"/>
+    </row>
+    <row r="142" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A142" s="6">
         <v>211</v>
       </c>
@@ -21228,9 +21801,13 @@
       <c r="AB142" s="6"/>
       <c r="AC142" s="6"/>
       <c r="AD142" s="6"/>
-      <c r="AE142" s="6"/>
-    </row>
-    <row r="143" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE142" s="6" t="str">
+        <f>IF(V142&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF142" s="6"/>
+    </row>
+    <row r="143" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A143" s="6">
         <v>212</v>
       </c>
@@ -21321,9 +21898,13 @@
       <c r="AB143" s="6"/>
       <c r="AC143" s="6"/>
       <c r="AD143" s="6"/>
-      <c r="AE143" s="6"/>
-    </row>
-    <row r="144" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE143" s="6" t="str">
+        <f>IF(V143&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF143" s="6"/>
+    </row>
+    <row r="144" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A144" s="6">
         <v>128</v>
       </c>
@@ -21412,9 +21993,13 @@
       <c r="AB144" s="6"/>
       <c r="AC144" s="6"/>
       <c r="AD144" s="6"/>
-      <c r="AE144" s="6"/>
-    </row>
-    <row r="145" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE144" s="6" t="str">
+        <f>IF(V144&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF144" s="6"/>
+    </row>
+    <row r="145" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A145" s="6">
         <v>200</v>
       </c>
@@ -21505,9 +22090,13 @@
       <c r="AB145" s="6"/>
       <c r="AC145" s="6"/>
       <c r="AD145" s="6"/>
-      <c r="AE145" s="6"/>
-    </row>
-    <row r="146" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE145" s="6" t="str">
+        <f>IF(V145&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF145" s="6"/>
+    </row>
+    <row r="146" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A146" s="6">
         <v>169</v>
       </c>
@@ -21598,9 +22187,13 @@
       <c r="AB146" s="6"/>
       <c r="AC146" s="6"/>
       <c r="AD146" s="6"/>
-      <c r="AE146" s="6"/>
-    </row>
-    <row r="147" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE146" s="6" t="str">
+        <f>IF(V146&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF146" s="6"/>
+    </row>
+    <row r="147" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A147" s="6">
         <v>132</v>
       </c>
@@ -21691,9 +22284,13 @@
       <c r="AB147" s="6"/>
       <c r="AC147" s="6"/>
       <c r="AD147" s="6"/>
-      <c r="AE147" s="6"/>
-    </row>
-    <row r="148" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE147" s="6" t="str">
+        <f>IF(V147&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF147" s="6"/>
+    </row>
+    <row r="148" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A148" s="6">
         <v>198</v>
       </c>
@@ -21782,9 +22379,13 @@
       <c r="AB148" s="6"/>
       <c r="AC148" s="6"/>
       <c r="AD148" s="6"/>
-      <c r="AE148" s="6"/>
-    </row>
-    <row r="149" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE148" s="6" t="str">
+        <f>IF(V148&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF148" s="6"/>
+    </row>
+    <row r="149" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A149" s="6">
         <v>199</v>
       </c>
@@ -21873,9 +22474,13 @@
       <c r="AB149" s="6"/>
       <c r="AC149" s="6"/>
       <c r="AD149" s="6"/>
-      <c r="AE149" s="6"/>
-    </row>
-    <row r="150" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE149" s="6" t="str">
+        <f>IF(V149&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF149" s="6"/>
+    </row>
+    <row r="150" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A150" s="6">
         <v>217</v>
       </c>
@@ -21966,9 +22571,13 @@
       <c r="AB150" s="6"/>
       <c r="AC150" s="6"/>
       <c r="AD150" s="6"/>
-      <c r="AE150" s="6"/>
-    </row>
-    <row r="151" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE150" s="6" t="str">
+        <f>IF(V150&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF150" s="6"/>
+    </row>
+    <row r="151" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A151" s="6">
         <v>162</v>
       </c>
@@ -22057,9 +22666,13 @@
       <c r="AB151" s="6"/>
       <c r="AC151" s="6"/>
       <c r="AD151" s="6"/>
-      <c r="AE151" s="6"/>
-    </row>
-    <row r="152" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE151" s="6" t="str">
+        <f>IF(V151&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF151" s="6"/>
+    </row>
+    <row r="152" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A152" s="6">
         <v>163</v>
       </c>
@@ -22148,9 +22761,13 @@
       <c r="AB152" s="6"/>
       <c r="AC152" s="6"/>
       <c r="AD152" s="6"/>
-      <c r="AE152" s="6"/>
-    </row>
-    <row r="153" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE152" s="6" t="str">
+        <f>IF(V152&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF152" s="6"/>
+    </row>
+    <row r="153" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A153" s="6">
         <v>161</v>
       </c>
@@ -22239,9 +22856,13 @@
       <c r="AB153" s="6"/>
       <c r="AC153" s="6"/>
       <c r="AD153" s="6"/>
-      <c r="AE153" s="6"/>
-    </row>
-    <row r="154" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE153" s="6" t="str">
+        <f>IF(V153&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF153" s="6"/>
+    </row>
+    <row r="154" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A154" s="6">
         <v>189</v>
       </c>
@@ -22330,9 +22951,13 @@
       <c r="AB154" s="6"/>
       <c r="AC154" s="6"/>
       <c r="AD154" s="6"/>
-      <c r="AE154" s="6"/>
-    </row>
-    <row r="155" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE154" s="6" t="str">
+        <f>IF(V154&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF154" s="6"/>
+    </row>
+    <row r="155" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A155" s="6">
         <v>220</v>
       </c>
@@ -22421,9 +23046,13 @@
       <c r="AB155" s="6"/>
       <c r="AC155" s="6"/>
       <c r="AD155" s="6"/>
-      <c r="AE155" s="6"/>
-    </row>
-    <row r="156" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE155" s="6" t="str">
+        <f>IF(V155&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF155" s="6"/>
+    </row>
+    <row r="156" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="5">
         <v>219</v>
       </c>
@@ -22516,11 +23145,14 @@
       <c r="AD156" s="5">
         <v>1</v>
       </c>
-      <c r="AE156" s="5"/>
-      <c r="AF156" s="2">
+      <c r="AE156" s="5" t="str">
+        <f>IF(V156&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF156" s="5"/>
+      <c r="AG156" s="2">
         <v>1</v>
       </c>
-      <c r="AG156"/>
       <c r="AH156"/>
       <c r="AI156"/>
       <c r="AJ156"/>
@@ -22559,8 +23191,9 @@
       <c r="BQ156"/>
       <c r="BR156"/>
       <c r="BS156"/>
-    </row>
-    <row r="157" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT156"/>
+    </row>
+    <row r="157" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A157" s="6">
         <v>221</v>
       </c>
@@ -22649,9 +23282,13 @@
       <c r="AB157" s="6"/>
       <c r="AC157" s="6"/>
       <c r="AD157" s="6"/>
-      <c r="AE157" s="6"/>
-    </row>
-    <row r="158" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE157" s="6">
+        <f>IF(V157&lt;5,1,"")</f>
+        <v>1</v>
+      </c>
+      <c r="AF157" s="6"/>
+    </row>
+    <row r="158" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A158" s="6">
         <v>129</v>
       </c>
@@ -22740,9 +23377,13 @@
       <c r="AB158" s="6"/>
       <c r="AC158" s="6"/>
       <c r="AD158" s="6"/>
-      <c r="AE158" s="6"/>
-    </row>
-    <row r="159" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE158" s="6" t="str">
+        <f>IF(V158&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF158" s="6"/>
+    </row>
+    <row r="159" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A159" s="6">
         <v>147</v>
       </c>
@@ -22833,9 +23474,13 @@
       <c r="AB159" s="6"/>
       <c r="AC159" s="6"/>
       <c r="AD159" s="6"/>
-      <c r="AE159" s="6"/>
-    </row>
-    <row r="160" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE159" s="6" t="str">
+        <f>IF(V159&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF159" s="6"/>
+    </row>
+    <row r="160" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A160" s="6">
         <v>148</v>
       </c>
@@ -22923,9 +23568,13 @@
       <c r="AB160" s="6"/>
       <c r="AC160" s="6"/>
       <c r="AD160" s="6"/>
-      <c r="AE160" s="6"/>
-    </row>
-    <row r="161" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE160" s="6" t="str">
+        <f>IF(V160&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF160" s="6"/>
+    </row>
+    <row r="161" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A161" s="6">
         <v>149</v>
       </c>
@@ -23014,9 +23663,13 @@
       <c r="AB161" s="6"/>
       <c r="AC161" s="6"/>
       <c r="AD161" s="6"/>
-      <c r="AE161" s="6"/>
-    </row>
-    <row r="162" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE161" s="6" t="str">
+        <f>IF(V161&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF161" s="6"/>
+    </row>
+    <row r="162" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A162" s="6">
         <v>141</v>
       </c>
@@ -23107,9 +23760,13 @@
       <c r="AB162" s="6"/>
       <c r="AC162" s="6"/>
       <c r="AD162" s="6"/>
-      <c r="AE162" s="6"/>
-    </row>
-    <row r="163" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE162" s="6" t="str">
+        <f>IF(V162&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF162" s="6"/>
+    </row>
+    <row r="163" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A163" s="6">
         <v>142</v>
       </c>
@@ -23198,9 +23855,13 @@
       <c r="AB163" s="6"/>
       <c r="AC163" s="6"/>
       <c r="AD163" s="6"/>
-      <c r="AE163" s="6"/>
-    </row>
-    <row r="164" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE163" s="6">
+        <f>IF(V163&lt;5,1,"")</f>
+        <v>1</v>
+      </c>
+      <c r="AF163" s="6"/>
+    </row>
+    <row r="164" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A164" s="6">
         <v>140</v>
       </c>
@@ -23289,9 +23950,13 @@
       <c r="AB164" s="6"/>
       <c r="AC164" s="6"/>
       <c r="AD164" s="6"/>
-      <c r="AE164" s="6"/>
-    </row>
-    <row r="165" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE164" s="6" t="str">
+        <f>IF(V164&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF164" s="6"/>
+    </row>
+    <row r="165" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A165" s="6">
         <v>138</v>
       </c>
@@ -23380,9 +24045,13 @@
       <c r="AB165" s="6"/>
       <c r="AC165" s="6"/>
       <c r="AD165" s="6"/>
-      <c r="AE165" s="6"/>
-    </row>
-    <row r="166" spans="1:71" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE165" s="6" t="str">
+        <f>IF(V165&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF165" s="6"/>
+    </row>
+    <row r="166" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A166" s="6">
         <v>139</v>
       </c>
@@ -23471,8 +24140,11 @@
       <c r="AB166" s="6"/>
       <c r="AC166" s="6"/>
       <c r="AD166" s="6"/>
-      <c r="AE166" s="6"/>
-      <c r="AF166"/>
+      <c r="AE166" s="6">
+        <f>IF(V166&lt;5,1,"")</f>
+        <v>1</v>
+      </c>
+      <c r="AF166" s="6"/>
       <c r="AG166"/>
       <c r="AH166"/>
       <c r="AI166"/>
@@ -23512,8 +24184,9 @@
       <c r="BQ166"/>
       <c r="BR166"/>
       <c r="BS166"/>
-    </row>
-    <row r="167" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT166"/>
+    </row>
+    <row r="167" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A167" s="6">
         <v>181</v>
       </c>
@@ -23602,9 +24275,13 @@
       <c r="AB167" s="6"/>
       <c r="AC167" s="6"/>
       <c r="AD167" s="6"/>
-      <c r="AE167" s="6"/>
-    </row>
-    <row r="168" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE167" s="6" t="str">
+        <f>IF(V167&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF167" s="6"/>
+    </row>
+    <row r="168" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A168" s="6">
         <v>202</v>
       </c>
@@ -23693,9 +24370,13 @@
       <c r="AB168" s="6"/>
       <c r="AC168" s="6"/>
       <c r="AD168" s="6"/>
-      <c r="AE168" s="6"/>
-    </row>
-    <row r="169" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE168" s="6" t="str">
+        <f>IF(V168&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF168" s="6"/>
+    </row>
+    <row r="169" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A169" s="6">
         <v>154</v>
       </c>
@@ -23786,9 +24467,13 @@
       <c r="AB169" s="6"/>
       <c r="AC169" s="6"/>
       <c r="AD169" s="6"/>
-      <c r="AE169" s="6"/>
-    </row>
-    <row r="170" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE169" s="6" t="str">
+        <f>IF(V169&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF169" s="6"/>
+    </row>
+    <row r="170" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A170" s="6">
         <v>197</v>
       </c>
@@ -23877,9 +24562,13 @@
       <c r="AB170" s="6"/>
       <c r="AC170" s="6"/>
       <c r="AD170" s="6"/>
-      <c r="AE170" s="6"/>
-    </row>
-    <row r="171" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE170" s="6" t="str">
+        <f>IF(V170&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF170" s="6"/>
+    </row>
+    <row r="171" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A171" s="6">
         <v>185</v>
       </c>
@@ -23968,9 +24657,13 @@
       <c r="AB171" s="6"/>
       <c r="AC171" s="6"/>
       <c r="AD171" s="6"/>
-      <c r="AE171" s="6"/>
-    </row>
-    <row r="172" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE171" s="6" t="str">
+        <f>IF(V171&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF171" s="6"/>
+    </row>
+    <row r="172" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A172" s="6">
         <v>192</v>
       </c>
@@ -24061,9 +24754,13 @@
       <c r="AB172" s="6"/>
       <c r="AC172" s="6"/>
       <c r="AD172" s="6"/>
-      <c r="AE172" s="6"/>
-    </row>
-    <row r="173" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE172" s="6" t="str">
+        <f>IF(V172&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF172" s="6"/>
+    </row>
+    <row r="173" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A173" s="6">
         <v>209</v>
       </c>
@@ -24152,9 +24849,13 @@
       <c r="AB173" s="6"/>
       <c r="AC173" s="6"/>
       <c r="AD173" s="6"/>
-      <c r="AE173" s="6"/>
-    </row>
-    <row r="174" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE173" s="6" t="str">
+        <f>IF(V173&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF173" s="6"/>
+    </row>
+    <row r="174" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A174" s="6">
         <v>210</v>
       </c>
@@ -24243,9 +24944,13 @@
       <c r="AB174" s="6"/>
       <c r="AC174" s="6"/>
       <c r="AD174" s="6"/>
-      <c r="AE174" s="6"/>
-    </row>
-    <row r="175" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE174" s="6" t="str">
+        <f>IF(V174&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF174" s="6"/>
+    </row>
+    <row r="175" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A175" s="6">
         <v>190</v>
       </c>
@@ -24336,9 +25041,13 @@
       <c r="AB175" s="6"/>
       <c r="AC175" s="6"/>
       <c r="AD175" s="6"/>
-      <c r="AE175" s="6"/>
-    </row>
-    <row r="176" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE175" s="6" t="str">
+        <f>IF(V175&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF175" s="6"/>
+    </row>
+    <row r="176" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A176" s="6">
         <v>150</v>
       </c>
@@ -24429,9 +25138,13 @@
       <c r="AB176" s="6"/>
       <c r="AC176" s="6"/>
       <c r="AD176" s="6"/>
-      <c r="AE176" s="6"/>
-    </row>
-    <row r="177" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE176" s="6" t="str">
+        <f>IF(V176&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF176" s="6"/>
+    </row>
+    <row r="177" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A177" s="6">
         <v>151</v>
       </c>
@@ -24522,9 +25235,13 @@
       <c r="AB177" s="6"/>
       <c r="AC177" s="6"/>
       <c r="AD177" s="6"/>
-      <c r="AE177" s="6"/>
-    </row>
-    <row r="178" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE177" s="6" t="str">
+        <f>IF(V177&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF177" s="6"/>
+    </row>
+    <row r="178" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A178" s="6">
         <v>177</v>
       </c>
@@ -24613,9 +25330,13 @@
       <c r="AB178" s="6"/>
       <c r="AC178" s="6"/>
       <c r="AD178" s="6"/>
-      <c r="AE178" s="6"/>
-    </row>
-    <row r="179" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE178" s="6" t="str">
+        <f>IF(V178&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF178" s="6"/>
+    </row>
+    <row r="179" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A179" s="6">
         <v>176</v>
       </c>
@@ -24706,9 +25427,13 @@
       <c r="AB179" s="6"/>
       <c r="AC179" s="6"/>
       <c r="AD179" s="6"/>
-      <c r="AE179" s="6"/>
-    </row>
-    <row r="180" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE179" s="6" t="str">
+        <f>IF(V179&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF179" s="6"/>
+    </row>
+    <row r="180" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A180" s="6">
         <v>175</v>
       </c>
@@ -24797,9 +25522,13 @@
       <c r="AB180" s="6"/>
       <c r="AC180" s="6"/>
       <c r="AD180" s="6"/>
-      <c r="AE180" s="6"/>
-    </row>
-    <row r="181" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE180" s="6" t="str">
+        <f>IF(V180&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF180" s="6"/>
+    </row>
+    <row r="181" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A181" s="6">
         <v>178</v>
       </c>
@@ -24890,9 +25619,13 @@
       <c r="AB181" s="6"/>
       <c r="AC181" s="6"/>
       <c r="AD181" s="6"/>
-      <c r="AE181" s="6"/>
-    </row>
-    <row r="182" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE181" s="6" t="str">
+        <f>IF(V181&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF181" s="6"/>
+    </row>
+    <row r="182" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A182" s="6">
         <v>201</v>
       </c>
@@ -24983,9 +25716,13 @@
       <c r="AB182" s="6"/>
       <c r="AC182" s="6"/>
       <c r="AD182" s="6"/>
-      <c r="AE182" s="6"/>
-    </row>
-    <row r="183" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE182" s="6" t="str">
+        <f>IF(V182&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF182" s="6"/>
+    </row>
+    <row r="183" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A183" s="6">
         <v>188</v>
       </c>
@@ -25076,9 +25813,13 @@
       <c r="AB183" s="6"/>
       <c r="AC183" s="6"/>
       <c r="AD183" s="6"/>
-      <c r="AE183" s="6"/>
-    </row>
-    <row r="184" spans="1:71" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE183" s="6" t="str">
+        <f>IF(V183&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF183" s="6"/>
+    </row>
+    <row r="184" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A184" s="6">
         <v>187</v>
       </c>
@@ -25169,8 +25910,11 @@
       <c r="AB184" s="6"/>
       <c r="AC184" s="6"/>
       <c r="AD184" s="6"/>
-      <c r="AE184" s="6"/>
-      <c r="AF184"/>
+      <c r="AE184" s="6" t="str">
+        <f>IF(V184&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF184" s="6"/>
       <c r="AG184"/>
       <c r="AH184"/>
       <c r="AI184"/>
@@ -25210,8 +25954,9 @@
       <c r="BQ184"/>
       <c r="BR184"/>
       <c r="BS184"/>
-    </row>
-    <row r="185" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT184"/>
+    </row>
+    <row r="185" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A185" s="6">
         <v>145</v>
       </c>
@@ -25302,9 +26047,13 @@
       <c r="AB185" s="6"/>
       <c r="AC185" s="6"/>
       <c r="AD185" s="6"/>
-      <c r="AE185" s="6"/>
-    </row>
-    <row r="186" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE185" s="6" t="str">
+        <f>IF(V185&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF185" s="6"/>
+    </row>
+    <row r="186" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A186" s="6">
         <v>223</v>
       </c>
@@ -25393,9 +26142,13 @@
       <c r="AB186" s="6"/>
       <c r="AC186" s="6"/>
       <c r="AD186" s="6"/>
-      <c r="AE186" s="6"/>
-    </row>
-    <row r="187" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE186" s="6" t="str">
+        <f>IF(V186&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF186" s="6"/>
+    </row>
+    <row r="187" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A187" s="6">
         <v>180</v>
       </c>
@@ -25484,9 +26237,13 @@
       <c r="AB187" s="6"/>
       <c r="AC187" s="6"/>
       <c r="AD187" s="6"/>
-      <c r="AE187" s="6"/>
-    </row>
-    <row r="188" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE187" s="6" t="str">
+        <f>IF(V187&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF187" s="6"/>
+    </row>
+    <row r="188" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A188" s="6">
         <v>179</v>
       </c>
@@ -25577,9 +26334,13 @@
       <c r="AB188" s="6"/>
       <c r="AC188" s="6"/>
       <c r="AD188" s="6"/>
-      <c r="AE188" s="6"/>
-    </row>
-    <row r="189" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE188" s="6" t="str">
+        <f>IF(V188&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF188" s="6"/>
+    </row>
+    <row r="189" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A189" s="6">
         <v>196</v>
       </c>
@@ -25668,9 +26429,13 @@
       <c r="AB189" s="6"/>
       <c r="AC189" s="6"/>
       <c r="AD189" s="6"/>
-      <c r="AE189" s="6"/>
-    </row>
-    <row r="190" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE189" s="6" t="str">
+        <f>IF(V189&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF189" s="6"/>
+    </row>
+    <row r="190" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A190" s="6">
         <v>131</v>
       </c>
@@ -25761,9 +26526,13 @@
       <c r="AB190" s="6"/>
       <c r="AC190" s="6"/>
       <c r="AD190" s="6"/>
-      <c r="AE190" s="6"/>
-    </row>
-    <row r="191" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE190" s="6" t="str">
+        <f>IF(V190&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF190" s="6"/>
+    </row>
+    <row r="191" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A191" s="6">
         <v>152</v>
       </c>
@@ -25854,9 +26623,13 @@
       <c r="AB191" s="6"/>
       <c r="AC191" s="6"/>
       <c r="AD191" s="6"/>
-      <c r="AE191" s="6"/>
-    </row>
-    <row r="192" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE191" s="6" t="str">
+        <f>IF(V191&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF191" s="6"/>
+    </row>
+    <row r="192" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A192" s="6">
         <v>153</v>
       </c>
@@ -25945,9 +26718,13 @@
       <c r="AB192" s="6"/>
       <c r="AC192" s="6"/>
       <c r="AD192" s="6"/>
-      <c r="AE192" s="6"/>
-    </row>
-    <row r="193" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE192" s="6" t="str">
+        <f>IF(V192&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF192" s="6"/>
+    </row>
+    <row r="193" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A193" s="6">
         <v>213</v>
       </c>
@@ -26038,9 +26815,13 @@
       <c r="AB193" s="6"/>
       <c r="AC193" s="6"/>
       <c r="AD193" s="6"/>
-      <c r="AE193" s="6"/>
-    </row>
-    <row r="194" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE193" s="6" t="str">
+        <f>IF(V193&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF193" s="6"/>
+    </row>
+    <row r="194" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A194" s="6">
         <v>193</v>
       </c>
@@ -26131,9 +26912,13 @@
       <c r="AB194" s="6"/>
       <c r="AC194" s="6"/>
       <c r="AD194" s="6"/>
-      <c r="AE194" s="6"/>
-    </row>
-    <row r="195" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE194" s="6" t="str">
+        <f>IF(V194&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF194" s="6"/>
+    </row>
+    <row r="195" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A195" s="6">
         <v>216</v>
       </c>
@@ -26224,9 +27009,13 @@
       <c r="AB195" s="6"/>
       <c r="AC195" s="6"/>
       <c r="AD195" s="6"/>
-      <c r="AE195" s="6"/>
-    </row>
-    <row r="196" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE195" s="6" t="str">
+        <f>IF(V195&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF195" s="6"/>
+    </row>
+    <row r="196" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A196" s="6">
         <v>208</v>
       </c>
@@ -26315,9 +27104,13 @@
       <c r="AB196" s="6"/>
       <c r="AC196" s="6"/>
       <c r="AD196" s="6"/>
-      <c r="AE196" s="6"/>
-    </row>
-    <row r="197" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE196" s="6" t="str">
+        <f>IF(V196&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF196" s="6"/>
+    </row>
+    <row r="197" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A197" s="6">
         <v>174</v>
       </c>
@@ -26408,9 +27201,13 @@
       <c r="AB197" s="6"/>
       <c r="AC197" s="6"/>
       <c r="AD197" s="6"/>
-      <c r="AE197" s="6"/>
-    </row>
-    <row r="198" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE197" s="6" t="str">
+        <f>IF(V197&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF197" s="6"/>
+    </row>
+    <row r="198" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A198" s="6">
         <v>173</v>
       </c>
@@ -26501,9 +27298,13 @@
       <c r="AB198" s="6"/>
       <c r="AC198" s="6"/>
       <c r="AD198" s="6"/>
-      <c r="AE198" s="6"/>
-    </row>
-    <row r="199" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE198" s="6" t="str">
+        <f>IF(V198&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF198" s="6"/>
+    </row>
+    <row r="199" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A199" s="6">
         <v>144</v>
       </c>
@@ -26592,9 +27393,13 @@
       <c r="AB199" s="6"/>
       <c r="AC199" s="6"/>
       <c r="AD199" s="6"/>
-      <c r="AE199" s="6"/>
-    </row>
-    <row r="200" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE199" s="6" t="str">
+        <f>IF(V199&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF199" s="6"/>
+    </row>
+    <row r="200" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A200" s="6">
         <v>159</v>
       </c>
@@ -26683,9 +27488,13 @@
       <c r="AB200" s="6"/>
       <c r="AC200" s="6"/>
       <c r="AD200" s="6"/>
-      <c r="AE200" s="6"/>
-    </row>
-    <row r="201" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE200" s="6" t="str">
+        <f>IF(V200&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF200" s="6"/>
+    </row>
+    <row r="201" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A201" s="6">
         <v>156</v>
       </c>
@@ -26776,9 +27585,13 @@
       <c r="AB201" s="6"/>
       <c r="AC201" s="6"/>
       <c r="AD201" s="6"/>
-      <c r="AE201" s="6"/>
-    </row>
-    <row r="202" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE201" s="6" t="str">
+        <f>IF(V201&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF201" s="6"/>
+    </row>
+    <row r="202" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A202" s="6">
         <v>158</v>
       </c>
@@ -26869,9 +27682,13 @@
       <c r="AB202" s="6"/>
       <c r="AC202" s="6"/>
       <c r="AD202" s="6"/>
-      <c r="AE202" s="6"/>
-    </row>
-    <row r="203" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE202" s="6" t="str">
+        <f>IF(V202&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF202" s="6"/>
+    </row>
+    <row r="203" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A203" s="6">
         <v>157</v>
       </c>
@@ -26962,9 +27779,13 @@
       <c r="AB203" s="6"/>
       <c r="AC203" s="6"/>
       <c r="AD203" s="6"/>
-      <c r="AE203" s="6"/>
-    </row>
-    <row r="204" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE203" s="6" t="str">
+        <f>IF(V203&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF203" s="6"/>
+    </row>
+    <row r="204" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A204" s="5">
         <v>155</v>
       </c>
@@ -27055,11 +27876,14 @@
       <c r="AD204" s="5">
         <v>1</v>
       </c>
-      <c r="AE204" s="5"/>
-      <c r="AF204" s="2">
+      <c r="AE204" s="5">
+        <f>IF(V204&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG204"/>
+      <c r="AF204" s="5"/>
+      <c r="AG204" s="2">
+        <v>1</v>
+      </c>
       <c r="AH204"/>
       <c r="AI204"/>
       <c r="AJ204"/>
@@ -27098,8 +27922,9 @@
       <c r="BQ204"/>
       <c r="BR204"/>
       <c r="BS204"/>
-    </row>
-    <row r="205" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT204"/>
+    </row>
+    <row r="205" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A205" s="6">
         <v>160</v>
       </c>
@@ -27190,9 +28015,13 @@
       <c r="AB205" s="6"/>
       <c r="AC205" s="6"/>
       <c r="AD205" s="6"/>
-      <c r="AE205" s="6"/>
-    </row>
-    <row r="206" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE205" s="6" t="str">
+        <f>IF(V205&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF205" s="6"/>
+    </row>
+    <row r="206" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A206" s="5">
         <v>9</v>
       </c>
@@ -27285,11 +28114,14 @@
       <c r="AD206" s="5">
         <v>1</v>
       </c>
-      <c r="AE206" s="5"/>
-      <c r="AF206" s="2">
+      <c r="AE206" s="5">
+        <f>IF(V206&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG206"/>
+      <c r="AF206" s="5"/>
+      <c r="AG206" s="2">
+        <v>1</v>
+      </c>
       <c r="AH206"/>
       <c r="AI206"/>
       <c r="AJ206"/>
@@ -27328,8 +28160,9 @@
       <c r="BQ206"/>
       <c r="BR206"/>
       <c r="BS206"/>
-    </row>
-    <row r="207" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT206"/>
+    </row>
+    <row r="207" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A207" s="6">
         <v>10</v>
       </c>
@@ -27418,9 +28251,13 @@
       <c r="AB207" s="6"/>
       <c r="AC207" s="6"/>
       <c r="AD207" s="6"/>
-      <c r="AE207" s="6"/>
-    </row>
-    <row r="208" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE207" s="6" t="str">
+        <f>IF(V207&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF207" s="6"/>
+    </row>
+    <row r="208" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A208" s="6">
         <v>8</v>
       </c>
@@ -27511,9 +28348,13 @@
       <c r="AB208" s="6"/>
       <c r="AC208" s="6"/>
       <c r="AD208" s="6"/>
-      <c r="AE208" s="6"/>
-    </row>
-    <row r="209" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE208" s="6" t="str">
+        <f>IF(V208&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF208" s="6"/>
+    </row>
+    <row r="209" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A209" s="6">
         <v>13</v>
       </c>
@@ -27604,9 +28445,13 @@
       <c r="AB209" s="6"/>
       <c r="AC209" s="6"/>
       <c r="AD209" s="6"/>
-      <c r="AE209" s="6"/>
-    </row>
-    <row r="210" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE209" s="6" t="str">
+        <f>IF(V209&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF209" s="6"/>
+    </row>
+    <row r="210" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A210" s="6">
         <v>125</v>
       </c>
@@ -27697,9 +28542,13 @@
       <c r="AB210" s="6"/>
       <c r="AC210" s="6"/>
       <c r="AD210" s="6"/>
-      <c r="AE210" s="6"/>
-    </row>
-    <row r="211" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE210" s="6" t="str">
+        <f>IF(V210&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF210" s="6"/>
+    </row>
+    <row r="211" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A211" s="5">
         <v>126</v>
       </c>
@@ -27790,11 +28639,14 @@
       <c r="AD211" s="5">
         <v>1</v>
       </c>
-      <c r="AE211" s="5"/>
-      <c r="AF211" s="2">
+      <c r="AE211" s="5">
+        <f>IF(V211&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG211"/>
+      <c r="AF211" s="5"/>
+      <c r="AG211" s="2">
+        <v>1</v>
+      </c>
       <c r="AH211"/>
       <c r="AI211"/>
       <c r="AJ211"/>
@@ -27833,8 +28685,9 @@
       <c r="BQ211"/>
       <c r="BR211"/>
       <c r="BS211"/>
-    </row>
-    <row r="212" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT211"/>
+    </row>
+    <row r="212" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A212" s="6">
         <v>127</v>
       </c>
@@ -27923,9 +28776,13 @@
       <c r="AB212" s="6"/>
       <c r="AC212" s="6"/>
       <c r="AD212" s="6"/>
-      <c r="AE212" s="6"/>
-    </row>
-    <row r="213" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE212" s="6" t="str">
+        <f>IF(V212&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF212" s="6"/>
+    </row>
+    <row r="213" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A213" s="6">
         <v>124</v>
       </c>
@@ -28016,9 +28873,13 @@
       <c r="AB213" s="6"/>
       <c r="AC213" s="6"/>
       <c r="AD213" s="6"/>
-      <c r="AE213" s="6"/>
-    </row>
-    <row r="214" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE213" s="6" t="str">
+        <f>IF(V213&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF213" s="6"/>
+    </row>
+    <row r="214" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A214" s="6">
         <v>122</v>
       </c>
@@ -28109,9 +28970,13 @@
       <c r="AB214" s="6"/>
       <c r="AC214" s="6"/>
       <c r="AD214" s="6"/>
-      <c r="AE214" s="6"/>
-    </row>
-    <row r="215" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE214" s="6" t="str">
+        <f>IF(V214&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF214" s="6"/>
+    </row>
+    <row r="215" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A215" s="6">
         <v>123</v>
       </c>
@@ -28202,9 +29067,13 @@
       <c r="AB215" s="6"/>
       <c r="AC215" s="6"/>
       <c r="AD215" s="6"/>
-      <c r="AE215" s="6"/>
-    </row>
-    <row r="216" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE215" s="6" t="str">
+        <f>IF(V215&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF215" s="6"/>
+    </row>
+    <row r="216" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A216" s="6">
         <v>4</v>
       </c>
@@ -28293,9 +29162,13 @@
       <c r="AB216" s="6"/>
       <c r="AC216" s="6"/>
       <c r="AD216" s="6"/>
-      <c r="AE216" s="6"/>
-    </row>
-    <row r="217" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE216" s="6">
+        <f>IF(V216&lt;5,1,"")</f>
+        <v>1</v>
+      </c>
+      <c r="AF216" s="6"/>
+    </row>
+    <row r="217" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A217" s="6">
         <v>2</v>
       </c>
@@ -28386,9 +29259,13 @@
       <c r="AB217" s="6"/>
       <c r="AC217" s="6"/>
       <c r="AD217" s="6"/>
-      <c r="AE217" s="6"/>
-    </row>
-    <row r="218" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE217" s="6" t="str">
+        <f>IF(V217&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF217" s="6"/>
+    </row>
+    <row r="218" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A218" s="6">
         <v>3</v>
       </c>
@@ -28479,9 +29356,13 @@
       <c r="AB218" s="6"/>
       <c r="AC218" s="6"/>
       <c r="AD218" s="6"/>
-      <c r="AE218" s="6"/>
-    </row>
-    <row r="219" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE218" s="6" t="str">
+        <f>IF(V218&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF218" s="6"/>
+    </row>
+    <row r="219" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A219" s="6">
         <v>5</v>
       </c>
@@ -28570,9 +29451,13 @@
       <c r="AB219" s="6"/>
       <c r="AC219" s="6"/>
       <c r="AD219" s="6"/>
-      <c r="AE219" s="6"/>
-    </row>
-    <row r="220" spans="1:71" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE219" s="6" t="str">
+        <f>IF(V219&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF219" s="6"/>
+    </row>
+    <row r="220" spans="1:72" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A220" s="6">
         <v>1</v>
       </c>
@@ -28663,8 +29548,11 @@
       <c r="AB220" s="6"/>
       <c r="AC220" s="6"/>
       <c r="AD220" s="6"/>
-      <c r="AE220" s="6"/>
-      <c r="AF220"/>
+      <c r="AE220" s="6" t="str">
+        <f>IF(V220&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF220" s="6"/>
       <c r="AG220"/>
       <c r="AH220"/>
       <c r="AI220"/>
@@ -28704,8 +29592,9 @@
       <c r="BQ220"/>
       <c r="BR220"/>
       <c r="BS220"/>
-    </row>
-    <row r="221" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT220"/>
+    </row>
+    <row r="221" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A221" s="5">
         <v>6</v>
       </c>
@@ -28796,11 +29685,14 @@
       </c>
       <c r="AC221" s="5"/>
       <c r="AD221" s="5"/>
-      <c r="AE221" s="5"/>
-      <c r="AF221" s="2">
+      <c r="AE221" s="5">
+        <f>IF(V221&lt;5,1,"")</f>
         <v>1</v>
       </c>
-      <c r="AG221"/>
+      <c r="AF221" s="5"/>
+      <c r="AG221" s="2">
+        <v>1</v>
+      </c>
       <c r="AH221"/>
       <c r="AI221"/>
       <c r="AJ221"/>
@@ -28839,8 +29731,9 @@
       <c r="BQ221"/>
       <c r="BR221"/>
       <c r="BS221"/>
-    </row>
-    <row r="222" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BT221"/>
+    </row>
+    <row r="222" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A222" s="5">
         <v>116</v>
       </c>
@@ -28933,11 +29826,14 @@
       <c r="AD222" s="5">
         <v>1</v>
       </c>
-      <c r="AE222" s="5"/>
-      <c r="AF222" s="2">
+      <c r="AE222" s="5" t="str">
+        <f>IF(V222&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF222" s="5"/>
+      <c r="AG222" s="2">
         <v>1</v>
       </c>
-      <c r="AG222"/>
       <c r="AH222"/>
       <c r="AI222"/>
       <c r="AJ222"/>
@@ -28976,8 +29872,9 @@
       <c r="BQ222"/>
       <c r="BR222"/>
       <c r="BS222"/>
-    </row>
-    <row r="223" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT222"/>
+    </row>
+    <row r="223" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A223" s="6">
         <v>115</v>
       </c>
@@ -29068,9 +29965,13 @@
       <c r="AB223" s="6"/>
       <c r="AC223" s="6"/>
       <c r="AD223" s="6"/>
-      <c r="AE223" s="6"/>
-    </row>
-    <row r="224" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE223" s="6" t="str">
+        <f>IF(V223&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF223" s="6"/>
+    </row>
+    <row r="224" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A224" s="6">
         <v>114</v>
       </c>
@@ -29159,9 +30060,13 @@
       <c r="AB224" s="6"/>
       <c r="AC224" s="6"/>
       <c r="AD224" s="6"/>
-      <c r="AE224" s="6"/>
-    </row>
-    <row r="225" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE224" s="6" t="str">
+        <f>IF(V224&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF224" s="6"/>
+    </row>
+    <row r="225" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A225" s="6">
         <v>112</v>
       </c>
@@ -29250,9 +30155,13 @@
       <c r="AB225" s="6"/>
       <c r="AC225" s="6"/>
       <c r="AD225" s="6"/>
-      <c r="AE225" s="6"/>
-    </row>
-    <row r="226" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE225" s="6" t="str">
+        <f>IF(V225&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF225" s="6"/>
+    </row>
+    <row r="226" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A226" s="6">
         <v>111</v>
       </c>
@@ -29341,9 +30250,13 @@
       <c r="AB226" s="6"/>
       <c r="AC226" s="6"/>
       <c r="AD226" s="6"/>
-      <c r="AE226" s="6"/>
-    </row>
-    <row r="227" spans="1:71" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE226" s="6" t="str">
+        <f>IF(V226&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF226" s="6"/>
+    </row>
+    <row r="227" spans="1:72" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A227" s="6">
         <v>113</v>
       </c>
@@ -29434,8 +30347,11 @@
       <c r="AB227" s="6"/>
       <c r="AC227" s="6"/>
       <c r="AD227" s="6"/>
-      <c r="AE227" s="6"/>
-      <c r="AF227"/>
+      <c r="AE227" s="6" t="str">
+        <f>IF(V227&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF227" s="6"/>
       <c r="AG227"/>
       <c r="AH227"/>
       <c r="AI227"/>
@@ -29475,8 +30391,9 @@
       <c r="BQ227"/>
       <c r="BR227"/>
       <c r="BS227"/>
-    </row>
-    <row r="228" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="BT227"/>
+    </row>
+    <row r="228" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A228" s="6">
         <v>110</v>
       </c>
@@ -29565,9 +30482,13 @@
       <c r="AB228" s="6"/>
       <c r="AC228" s="6"/>
       <c r="AD228" s="6"/>
-      <c r="AE228" s="6"/>
-    </row>
-    <row r="229" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="AE228" s="6" t="str">
+        <f>IF(V228&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF228" s="6"/>
+    </row>
+    <row r="229" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A229" s="6">
         <v>7</v>
       </c>
@@ -29658,14 +30579,18 @@
       <c r="AB229" s="6"/>
       <c r="AC229" s="6"/>
       <c r="AD229" s="6"/>
-      <c r="AE229" s="6"/>
+      <c r="AE229" s="6" t="str">
+        <f>IF(V229&lt;5,1,"")</f>
+        <v/>
+      </c>
+      <c r="AF229" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE229">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF229">
     <sortCondition ref="J2:J229"/>
     <sortCondition ref="E2:E229"/>
   </sortState>
-  <conditionalFormatting sqref="A2:XFD21 A22:AA22 AC22:XFD22 A23:XFD229">
+  <conditionalFormatting sqref="A22:AA22 AC22:XFD22 A23:XFD229 A2:XFD21">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>"$AA=test"</formula>
     </cfRule>

</xml_diff>